<commit_message>
teabag data upload and start of r analysis
</commit_message>
<xml_diff>
--- a/Tea_bag_analysis/Tea_bag_decomposition_non-woven.xlsx
+++ b/Tea_bag_analysis/Tea_bag_decomposition_non-woven.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfilewych1/Documents/GitHub/Garibaldi/Tea_bag_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA67723-9355-E344-95D6-EC17B5EB75F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35FFA52-9202-3046-B489-136874E24272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="760" windowWidth="29780" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
     <definedName name="Wri">data!$J:$J</definedName>
     <definedName name="Wt">data!$R:$R</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -61,6 +61,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="412">
   <si>
     <t xml:space="preserve">&lt;TBI DATA FORM&gt; </t>
   </si>
@@ -2173,15 +2174,6 @@
     <t>inctime</t>
   </si>
   <si>
-    <t>July 20 2022</t>
-  </si>
-  <si>
-    <t>July 19 2022</t>
-  </si>
-  <si>
-    <t>July 21 2022</t>
-  </si>
-  <si>
     <t>Site (as labeled)</t>
   </si>
   <si>
@@ -2235,6 +2227,9 @@
   <si>
     <t>PR-24</t>
   </si>
+  <si>
+    <t>NA</t>
+  </si>
 </sst>
 </file>
 
@@ -2247,7 +2242,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="[$-409]d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2336,8 +2331,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2390,12 +2399,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEEF7E3"/>
-        <bgColor rgb="FFEEF7E3"/>
       </patternFill>
     </fill>
     <fill>
@@ -2835,7 +2838,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -3086,29 +3089,71 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3117,51 +3162,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3435,8 +3441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="G112" sqref="G112"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="V61" sqref="V61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3796,12 +3802,12 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
-      <c r="B12" s="172" t="s">
+      <c r="B12" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="141"/>
-      <c r="D12" s="141"/>
-      <c r="E12" s="141"/>
+      <c r="C12" s="136"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="136"/>
       <c r="F12" s="14"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
@@ -3826,12 +3832,12 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
-      <c r="B13" s="167" t="s">
+      <c r="B13" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="168"/>
-      <c r="D13" s="168"/>
-      <c r="E13" s="168"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="138"/>
       <c r="F13" s="17"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
@@ -3856,12 +3862,12 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="168"/>
+      <c r="C14" s="138"/>
+      <c r="D14" s="138"/>
+      <c r="E14" s="138"/>
       <c r="F14" s="18"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -3886,12 +3892,12 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
-      <c r="B15" s="167" t="s">
+      <c r="B15" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="168"/>
-      <c r="D15" s="168"/>
-      <c r="E15" s="168"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="138"/>
+      <c r="E15" s="138"/>
       <c r="F15" s="18"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -3916,12 +3922,12 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
-      <c r="B16" s="167" t="s">
+      <c r="B16" s="137" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="168"/>
-      <c r="D16" s="168"/>
-      <c r="E16" s="168"/>
+      <c r="C16" s="138"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="138"/>
       <c r="F16" s="18"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -3946,12 +3952,12 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
-      <c r="B17" s="167" t="s">
+      <c r="B17" s="137" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="168"/>
-      <c r="D17" s="168"/>
-      <c r="E17" s="168"/>
+      <c r="C17" s="138"/>
+      <c r="D17" s="138"/>
+      <c r="E17" s="138"/>
       <c r="F17" s="18"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -3976,12 +3982,12 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
-      <c r="B18" s="167" t="s">
+      <c r="B18" s="137" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="168"/>
-      <c r="D18" s="168"/>
-      <c r="E18" s="168"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="138"/>
       <c r="F18" s="18"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -4006,12 +4012,12 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
-      <c r="B19" s="171" t="s">
+      <c r="B19" s="139" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="144"/>
-      <c r="D19" s="144"/>
-      <c r="E19" s="144"/>
+      <c r="C19" s="140"/>
+      <c r="D19" s="140"/>
+      <c r="E19" s="140"/>
       <c r="F19" s="20"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -4156,12 +4162,12 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
-      <c r="B24" s="172" t="s">
+      <c r="B24" s="135" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="141"/>
-      <c r="D24" s="141"/>
-      <c r="E24" s="141"/>
+      <c r="C24" s="136"/>
+      <c r="D24" s="136"/>
+      <c r="E24" s="136"/>
       <c r="F24" s="23">
         <v>0.84199999999999997</v>
       </c>
@@ -4188,12 +4194,12 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
-      <c r="B25" s="167" t="s">
+      <c r="B25" s="137" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="168"/>
-      <c r="D25" s="168"/>
-      <c r="E25" s="168"/>
+      <c r="C25" s="138"/>
+      <c r="D25" s="138"/>
+      <c r="E25" s="138"/>
       <c r="F25" s="24">
         <v>0.55200000000000005</v>
       </c>
@@ -4220,12 +4226,12 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
-      <c r="B26" s="167" t="s">
+      <c r="B26" s="137" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="168"/>
-      <c r="D26" s="168"/>
-      <c r="E26" s="168"/>
+      <c r="C26" s="138"/>
+      <c r="D26" s="138"/>
+      <c r="E26" s="138"/>
       <c r="F26" s="25">
         <v>0.2494625</v>
       </c>
@@ -4252,12 +4258,12 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
-      <c r="B27" s="167" t="s">
+      <c r="B27" s="137" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="168"/>
-      <c r="D27" s="168"/>
-      <c r="E27" s="168"/>
+      <c r="C27" s="138"/>
+      <c r="D27" s="138"/>
+      <c r="E27" s="138"/>
       <c r="F27" s="26"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -4312,12 +4318,12 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
-      <c r="B29" s="167" t="s">
+      <c r="B29" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="168"/>
-      <c r="D29" s="168"/>
-      <c r="E29" s="168"/>
+      <c r="C29" s="138"/>
+      <c r="D29" s="138"/>
+      <c r="E29" s="138"/>
       <c r="F29" s="26"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -4436,13 +4442,13 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
-      <c r="B33" s="169" t="s">
+      <c r="B33" s="141" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="163"/>
-      <c r="D33" s="163"/>
-      <c r="E33" s="163"/>
-      <c r="F33" s="164"/>
+      <c r="C33" s="142"/>
+      <c r="D33" s="142"/>
+      <c r="E33" s="142"/>
+      <c r="F33" s="143"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
@@ -4466,13 +4472,13 @@
     </row>
     <row r="34" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9"/>
-      <c r="B34" s="170" t="s">
+      <c r="B34" s="144" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="149"/>
-      <c r="D34" s="149"/>
-      <c r="E34" s="149"/>
-      <c r="F34" s="150"/>
+      <c r="C34" s="145"/>
+      <c r="D34" s="145"/>
+      <c r="E34" s="145"/>
+      <c r="F34" s="146"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
@@ -4614,16 +4620,16 @@
     </row>
     <row r="39" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
-      <c r="B39" s="161" t="s">
+      <c r="B39" s="147" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="144"/>
-      <c r="D39" s="144"/>
-      <c r="E39" s="162" t="s">
+      <c r="C39" s="140"/>
+      <c r="D39" s="140"/>
+      <c r="E39" s="148" t="s">
         <v>38</v>
       </c>
-      <c r="F39" s="163"/>
-      <c r="G39" s="164"/>
+      <c r="F39" s="142"/>
+      <c r="G39" s="143"/>
       <c r="H39" s="30" t="s">
         <v>39</v>
       </c>
@@ -4631,16 +4637,16 @@
       <c r="J39" s="31"/>
       <c r="K39" s="31"/>
       <c r="L39" s="23"/>
-      <c r="M39" s="142" t="s">
+      <c r="M39" s="149" t="s">
         <v>40</v>
       </c>
-      <c r="N39" s="141"/>
-      <c r="O39" s="141"/>
-      <c r="P39" s="141"/>
-      <c r="Q39" s="141"/>
-      <c r="R39" s="141"/>
-      <c r="S39" s="141"/>
-      <c r="T39" s="155"/>
+      <c r="N39" s="136"/>
+      <c r="O39" s="136"/>
+      <c r="P39" s="136"/>
+      <c r="Q39" s="136"/>
+      <c r="R39" s="136"/>
+      <c r="S39" s="136"/>
+      <c r="T39" s="150"/>
       <c r="U39" s="9"/>
       <c r="V39" s="9"/>
       <c r="W39" s="9"/>
@@ -4650,15 +4656,15 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
-      <c r="B40" s="165" t="s">
+      <c r="B40" s="151" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="163"/>
-      <c r="D40" s="164"/>
-      <c r="E40" s="166" t="s">
+      <c r="C40" s="142"/>
+      <c r="D40" s="143"/>
+      <c r="E40" s="152" t="s">
         <v>42</v>
       </c>
-      <c r="F40" s="163"/>
+      <c r="F40" s="142"/>
       <c r="G40" s="33" t="s">
         <v>43</v>
       </c>
@@ -4710,13 +4716,13 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
-      <c r="B41" s="158" t="s">
+      <c r="B41" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="146"/>
-      <c r="D41" s="147"/>
-      <c r="E41" s="156"/>
-      <c r="F41" s="157"/>
+      <c r="C41" s="156"/>
+      <c r="D41" s="157"/>
+      <c r="E41" s="153"/>
+      <c r="F41" s="154"/>
       <c r="G41" s="37"/>
       <c r="H41" s="38"/>
       <c r="I41" s="39"/>
@@ -4740,13 +4746,13 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9"/>
-      <c r="B42" s="135" t="s">
+      <c r="B42" s="158" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="136"/>
-      <c r="D42" s="137"/>
-      <c r="E42" s="159"/>
-      <c r="F42" s="139"/>
+      <c r="C42" s="159"/>
+      <c r="D42" s="160"/>
+      <c r="E42" s="161"/>
+      <c r="F42" s="162"/>
       <c r="G42" s="41"/>
       <c r="H42" s="38"/>
       <c r="I42" s="39"/>
@@ -4770,11 +4776,11 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9"/>
-      <c r="B43" s="135"/>
-      <c r="C43" s="136"/>
-      <c r="D43" s="137"/>
-      <c r="E43" s="160"/>
-      <c r="F43" s="139"/>
+      <c r="B43" s="158"/>
+      <c r="C43" s="159"/>
+      <c r="D43" s="160"/>
+      <c r="E43" s="163"/>
+      <c r="F43" s="162"/>
       <c r="G43" s="41"/>
       <c r="H43" s="38"/>
       <c r="I43" s="39"/>
@@ -4798,11 +4804,11 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
-      <c r="B44" s="135"/>
-      <c r="C44" s="136"/>
-      <c r="D44" s="137"/>
-      <c r="E44" s="138"/>
-      <c r="F44" s="139"/>
+      <c r="B44" s="158"/>
+      <c r="C44" s="159"/>
+      <c r="D44" s="160"/>
+      <c r="E44" s="164"/>
+      <c r="F44" s="162"/>
       <c r="G44" s="18"/>
       <c r="H44" s="38"/>
       <c r="I44" s="39"/>
@@ -4826,11 +4832,11 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
-      <c r="B45" s="135"/>
-      <c r="C45" s="136"/>
-      <c r="D45" s="137"/>
-      <c r="E45" s="138"/>
-      <c r="F45" s="139"/>
+      <c r="B45" s="158"/>
+      <c r="C45" s="159"/>
+      <c r="D45" s="160"/>
+      <c r="E45" s="164"/>
+      <c r="F45" s="162"/>
       <c r="G45" s="18"/>
       <c r="H45" s="38"/>
       <c r="I45" s="39"/>
@@ -4854,11 +4860,11 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9"/>
-      <c r="B46" s="135"/>
-      <c r="C46" s="136"/>
-      <c r="D46" s="137"/>
-      <c r="E46" s="138"/>
-      <c r="F46" s="139"/>
+      <c r="B46" s="158"/>
+      <c r="C46" s="159"/>
+      <c r="D46" s="160"/>
+      <c r="E46" s="164"/>
+      <c r="F46" s="162"/>
       <c r="G46" s="18"/>
       <c r="H46" s="38"/>
       <c r="I46" s="39"/>
@@ -4882,11 +4888,11 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9"/>
-      <c r="B47" s="151"/>
-      <c r="C47" s="149"/>
-      <c r="D47" s="150"/>
-      <c r="E47" s="152"/>
-      <c r="F47" s="153"/>
+      <c r="B47" s="169"/>
+      <c r="C47" s="145"/>
+      <c r="D47" s="146"/>
+      <c r="E47" s="170"/>
+      <c r="F47" s="171"/>
       <c r="G47" s="20"/>
       <c r="H47" s="42"/>
       <c r="I47" s="43"/>
@@ -4998,20 +5004,20 @@
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
-      <c r="B51" s="140" t="s">
+      <c r="B51" s="165" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="141"/>
-      <c r="D51" s="141"/>
-      <c r="E51" s="141"/>
-      <c r="F51" s="154" t="s">
+      <c r="C51" s="136"/>
+      <c r="D51" s="136"/>
+      <c r="E51" s="136"/>
+      <c r="F51" s="172" t="s">
         <v>62</v>
       </c>
-      <c r="G51" s="141"/>
-      <c r="H51" s="141"/>
-      <c r="I51" s="141"/>
-      <c r="J51" s="141"/>
-      <c r="K51" s="155"/>
+      <c r="G51" s="136"/>
+      <c r="H51" s="136"/>
+      <c r="I51" s="136"/>
+      <c r="J51" s="136"/>
+      <c r="K51" s="150"/>
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
       <c r="N51" s="9"/>
@@ -5030,20 +5036,20 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9"/>
-      <c r="B52" s="142" t="s">
+      <c r="B52" s="149" t="s">
         <v>63</v>
       </c>
-      <c r="C52" s="141"/>
-      <c r="D52" s="141"/>
-      <c r="E52" s="141"/>
-      <c r="F52" s="145" t="s">
+      <c r="C52" s="136"/>
+      <c r="D52" s="136"/>
+      <c r="E52" s="136"/>
+      <c r="F52" s="167" t="s">
         <v>64</v>
       </c>
-      <c r="G52" s="146"/>
-      <c r="H52" s="146"/>
-      <c r="I52" s="146"/>
-      <c r="J52" s="146"/>
-      <c r="K52" s="147"/>
+      <c r="G52" s="156"/>
+      <c r="H52" s="156"/>
+      <c r="I52" s="156"/>
+      <c r="J52" s="156"/>
+      <c r="K52" s="157"/>
       <c r="L52" s="9"/>
       <c r="M52" s="9"/>
       <c r="N52" s="9"/>
@@ -5062,20 +5068,20 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9"/>
-      <c r="B53" s="143" t="s">
+      <c r="B53" s="166" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="144"/>
-      <c r="D53" s="144"/>
-      <c r="E53" s="144"/>
-      <c r="F53" s="148" t="s">
+      <c r="C53" s="140"/>
+      <c r="D53" s="140"/>
+      <c r="E53" s="140"/>
+      <c r="F53" s="168" t="s">
         <v>66</v>
       </c>
-      <c r="G53" s="149"/>
-      <c r="H53" s="149"/>
-      <c r="I53" s="149"/>
-      <c r="J53" s="149"/>
-      <c r="K53" s="150"/>
+      <c r="G53" s="145"/>
+      <c r="H53" s="145"/>
+      <c r="I53" s="145"/>
+      <c r="J53" s="145"/>
+      <c r="K53" s="146"/>
       <c r="L53" s="9"/>
       <c r="M53" s="9"/>
       <c r="N53" s="9"/>
@@ -5594,8 +5600,8 @@
       <c r="E63" s="59">
         <v>1</v>
       </c>
-      <c r="F63" s="132" t="s">
-        <v>393</v>
+      <c r="F63" s="173">
+        <v>44762</v>
       </c>
       <c r="G63" s="60">
         <v>2.0802999999999998</v>
@@ -5611,34 +5617,34 @@
         <f t="shared" si="1"/>
         <v>1.9797175</v>
       </c>
-      <c r="K63" s="61"/>
+      <c r="K63" s="61">
+        <v>45105</v>
+      </c>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
-      <c r="N63" s="58"/>
-      <c r="O63" s="58"/>
-      <c r="P63" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q63" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R63" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S63" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T63" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U63" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N63" s="177">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="O63" s="177">
+        <v>1.694</v>
+      </c>
+      <c r="P63" s="177">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="Q63" s="177">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="R63" s="177">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="S63" s="177">
+        <v>343</v>
+      </c>
+      <c r="T63" s="177">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="U63" s="177">
+        <v>1.298408996E-3</v>
       </c>
       <c r="V63" s="1"/>
       <c r="W63" s="1"/>
@@ -5660,8 +5666,8 @@
       <c r="E64" s="59">
         <v>1</v>
       </c>
-      <c r="F64" s="133" t="s">
-        <v>393</v>
+      <c r="F64" s="173">
+        <v>44762</v>
       </c>
       <c r="G64" s="60">
         <v>2.0937999999999999</v>
@@ -5677,34 +5683,34 @@
         <f t="shared" si="1"/>
         <v>2.1256975000000002</v>
       </c>
-      <c r="K64" s="61"/>
+      <c r="K64" s="61">
+        <v>45105</v>
+      </c>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
-      <c r="N64" s="58"/>
-      <c r="O64" s="58"/>
-      <c r="P64" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q64" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R64" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S64" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T64" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U64" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N64" s="177">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="O64" s="177">
+        <v>1.643</v>
+      </c>
+      <c r="P64" s="177">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="Q64" s="177">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="R64" s="177">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="S64" s="177">
+        <v>343</v>
+      </c>
+      <c r="T64" s="177">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="U64" s="177">
+        <v>2.835042937E-3</v>
       </c>
       <c r="V64" s="1"/>
       <c r="W64" s="1"/>
@@ -5726,8 +5732,8 @@
       <c r="E65" s="59">
         <v>1</v>
       </c>
-      <c r="F65" s="132" t="s">
-        <v>393</v>
+      <c r="F65" s="173">
+        <v>44762</v>
       </c>
       <c r="G65" s="60">
         <v>2.10093</v>
@@ -5743,34 +5749,34 @@
         <f t="shared" si="1"/>
         <v>2.0702975000000001</v>
       </c>
-      <c r="K65" s="61"/>
+      <c r="K65" s="61">
+        <v>45105</v>
+      </c>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
-      <c r="N65" s="58"/>
-      <c r="O65" s="58"/>
-      <c r="P65" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q65" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R65" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S65" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T65" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U65" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N65" s="177" t="s">
+        <v>411</v>
+      </c>
+      <c r="O65" s="177">
+        <v>1.68</v>
+      </c>
+      <c r="P65" s="178" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q65" s="178" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R65" s="177">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="S65" s="177">
+        <v>343</v>
+      </c>
+      <c r="T65" s="178" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="U65" s="178" t="e">
+        <v>#VALUE!</v>
       </c>
       <c r="V65" s="1"/>
       <c r="W65" s="1"/>
@@ -5792,8 +5798,8 @@
       <c r="E66" s="59">
         <v>1</v>
       </c>
-      <c r="F66" s="133" t="s">
-        <v>393</v>
+      <c r="F66" s="173">
+        <v>44762</v>
       </c>
       <c r="G66" s="60">
         <v>2.0602</v>
@@ -5809,34 +5815,34 @@
         <f t="shared" si="1"/>
         <v>1.9846474999999999</v>
       </c>
-      <c r="K66" s="61"/>
+      <c r="K66" s="61">
+        <v>45105</v>
+      </c>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
-      <c r="N66" s="58"/>
-      <c r="O66" s="58"/>
-      <c r="P66" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q66" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R66" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S66" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T66" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U66" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N66" s="177">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="O66" s="177">
+        <v>1.6459999999999999</v>
+      </c>
+      <c r="P66" s="177">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="Q66" s="177">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="R66" s="177">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="S66" s="177">
+        <v>343</v>
+      </c>
+      <c r="T66" s="177">
+        <v>0.309</v>
+      </c>
+      <c r="U66" s="177">
+        <v>1.7284795770000001E-3</v>
       </c>
       <c r="V66" s="1"/>
       <c r="W66" s="1"/>
@@ -5858,8 +5864,8 @@
       <c r="E67" s="59">
         <v>1</v>
       </c>
-      <c r="F67" s="132" t="s">
-        <v>393</v>
+      <c r="F67" s="173">
+        <v>44762</v>
       </c>
       <c r="G67" s="60">
         <v>2.0886999999999998</v>
@@ -5875,34 +5881,34 @@
         <f t="shared" si="1"/>
         <v>2.0681875000000001</v>
       </c>
-      <c r="K67" s="61"/>
+      <c r="K67" s="61">
+        <v>45105</v>
+      </c>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
-      <c r="N67" s="58"/>
-      <c r="O67" s="58"/>
-      <c r="P67" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q67" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R67" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S67" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T67" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U67" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N67" s="177">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="O67" s="177">
+        <v>1.657</v>
+      </c>
+      <c r="P67" s="177">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="Q67" s="177">
+        <v>0.377</v>
+      </c>
+      <c r="R67" s="177">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="S67" s="177">
+        <v>343</v>
+      </c>
+      <c r="T67" s="177">
+        <v>0.317</v>
+      </c>
+      <c r="U67" s="177">
+        <v>2.1862586060000001E-3</v>
       </c>
       <c r="V67" s="1"/>
       <c r="W67" s="1"/>
@@ -5924,8 +5930,8 @@
       <c r="E68" s="59">
         <v>1</v>
       </c>
-      <c r="F68" s="133" t="s">
-        <v>393</v>
+      <c r="F68" s="173">
+        <v>44762</v>
       </c>
       <c r="G68" s="60">
         <v>2.0000399999999998</v>
@@ -5941,34 +5947,34 @@
         <f t="shared" si="1"/>
         <v>2.0950175</v>
       </c>
-      <c r="K68" s="61"/>
+      <c r="K68" s="61">
+        <v>45105</v>
+      </c>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
-      <c r="N68" s="58"/>
-      <c r="O68" s="58"/>
-      <c r="P68" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q68" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R68" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S68" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T68" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U68" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N68" s="177" t="s">
+        <v>411</v>
+      </c>
+      <c r="O68" s="177">
+        <v>1.508</v>
+      </c>
+      <c r="P68" s="178" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q68" s="178" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R68" s="177">
+        <v>0.72</v>
+      </c>
+      <c r="S68" s="177">
+        <v>343</v>
+      </c>
+      <c r="T68" s="178" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="U68" s="178" t="e">
+        <v>#VALUE!</v>
       </c>
       <c r="V68" s="1"/>
       <c r="W68" s="1"/>
@@ -5990,8 +5996,8 @@
       <c r="E69" s="59">
         <v>1</v>
       </c>
-      <c r="F69" s="132" t="s">
-        <v>393</v>
+      <c r="F69" s="173">
+        <v>44762</v>
       </c>
       <c r="G69" s="60">
         <v>1.8488500000000001</v>
@@ -6007,34 +6013,34 @@
         <f t="shared" si="1"/>
         <v>2.0785274999999999</v>
       </c>
-      <c r="K69" s="61"/>
+      <c r="K69" s="61">
+        <v>45105</v>
+      </c>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
-      <c r="N69" s="58"/>
-      <c r="O69" s="58"/>
-      <c r="P69" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q69" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R69" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S69" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T69" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U69" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N69" s="177">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="O69" s="177">
+        <v>1.625</v>
+      </c>
+      <c r="P69" s="177">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="Q69" s="177">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="R69" s="177">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="S69" s="177">
+        <v>343</v>
+      </c>
+      <c r="T69" s="177">
+        <v>0.38</v>
+      </c>
+      <c r="U69" s="177">
+        <v>2.9622584220000002E-3</v>
       </c>
       <c r="V69" s="1"/>
       <c r="W69" s="1"/>
@@ -6056,8 +6062,8 @@
       <c r="E70" s="59">
         <v>1</v>
       </c>
-      <c r="F70" s="133" t="s">
-        <v>393</v>
+      <c r="F70" s="173">
+        <v>44762</v>
       </c>
       <c r="G70" s="60">
         <v>2.09538</v>
@@ -6073,34 +6079,34 @@
         <f t="shared" si="1"/>
         <v>1.9935575000000001</v>
       </c>
-      <c r="K70" s="61"/>
+      <c r="K70" s="61">
+        <v>45105</v>
+      </c>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
-      <c r="N70" s="58"/>
-      <c r="O70" s="58"/>
-      <c r="P70" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q70" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R70" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S70" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T70" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U70" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N70" s="177">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="O70" s="177">
+        <v>1.4710000000000001</v>
+      </c>
+      <c r="P70" s="177">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="Q70" s="177">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="R70" s="177">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="S70" s="177">
+        <v>343</v>
+      </c>
+      <c r="T70" s="177">
+        <v>0.31</v>
+      </c>
+      <c r="U70" s="177">
+        <v>3.3948293279999998E-3</v>
       </c>
       <c r="V70" s="1"/>
       <c r="W70" s="1"/>
@@ -6122,8 +6128,8 @@
       <c r="E71" s="59">
         <v>1</v>
       </c>
-      <c r="F71" s="132" t="s">
-        <v>394</v>
+      <c r="F71" s="173">
+        <v>44761</v>
       </c>
       <c r="G71" s="60">
         <v>2.0102099999999998</v>
@@ -6139,34 +6145,34 @@
         <f t="shared" si="1"/>
         <v>2.0901274999999999</v>
       </c>
-      <c r="K71" s="61"/>
+      <c r="K71" s="61">
+        <v>45105</v>
+      </c>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
-      <c r="N71" s="58"/>
-      <c r="O71" s="58"/>
-      <c r="P71" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q71" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R71" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S71" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T71" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U71" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N71" s="177">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="O71" s="177">
+        <v>1.538</v>
+      </c>
+      <c r="P71" s="177">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="Q71" s="177">
+        <v>0.379</v>
+      </c>
+      <c r="R71" s="177">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="S71" s="177">
+        <v>344</v>
+      </c>
+      <c r="T71" s="177">
+        <v>0.314</v>
+      </c>
+      <c r="U71" s="177">
+        <v>3.4719792519999999E-3</v>
       </c>
       <c r="V71" s="1"/>
       <c r="W71" s="1"/>
@@ -6188,8 +6194,8 @@
       <c r="E72" s="59">
         <v>1</v>
       </c>
-      <c r="F72" s="133" t="s">
-        <v>394</v>
+      <c r="F72" s="173">
+        <v>44761</v>
       </c>
       <c r="G72" s="60">
         <v>1.9446099999999999</v>
@@ -6205,34 +6211,34 @@
         <f t="shared" si="1"/>
         <v>2.1281375000000002</v>
       </c>
-      <c r="K72" s="61"/>
+      <c r="K72" s="61">
+        <v>45105</v>
+      </c>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
-      <c r="N72" s="58"/>
-      <c r="O72" s="58"/>
-      <c r="P72" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q72" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R72" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S72" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T72" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U72" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N72" s="177" t="s">
+        <v>411</v>
+      </c>
+      <c r="O72" s="177">
+        <v>1.504</v>
+      </c>
+      <c r="P72" s="178" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q72" s="178" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R72" s="177">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="S72" s="177">
+        <v>344</v>
+      </c>
+      <c r="T72" s="178" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="U72" s="178" t="e">
+        <v>#VALUE!</v>
       </c>
       <c r="V72" s="1"/>
       <c r="W72" s="1"/>
@@ -6254,8 +6260,8 @@
       <c r="E73" s="59">
         <v>1</v>
       </c>
-      <c r="F73" s="132" t="s">
-        <v>394</v>
+      <c r="F73" s="173">
+        <v>44761</v>
       </c>
       <c r="G73" s="60">
         <v>1.9706300000000001</v>
@@ -6271,34 +6277,34 @@
         <f t="shared" si="1"/>
         <v>2.0530675</v>
       </c>
-      <c r="K73" s="61"/>
+      <c r="K73" s="61">
+        <v>45105</v>
+      </c>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
-      <c r="N73" s="58"/>
-      <c r="O73" s="58"/>
-      <c r="P73" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q73" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R73" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S73" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T73" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U73" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N73" s="177">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="O73" s="177">
+        <v>1.6679999999999999</v>
+      </c>
+      <c r="P73" s="177">
+        <v>0.61</v>
+      </c>
+      <c r="Q73" s="177">
+        <v>0.4</v>
+      </c>
+      <c r="R73" s="177">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="S73" s="177">
+        <v>344</v>
+      </c>
+      <c r="T73" s="177">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="U73" s="177">
+        <v>1.841943165E-3</v>
       </c>
       <c r="V73" s="1"/>
       <c r="W73" s="1"/>
@@ -6320,8 +6326,8 @@
       <c r="E74" s="59">
         <v>1</v>
       </c>
-      <c r="F74" s="133" t="s">
-        <v>394</v>
+      <c r="F74" s="173">
+        <v>44761</v>
       </c>
       <c r="G74" s="60">
         <v>2.12982</v>
@@ -6337,34 +6343,34 @@
         <f t="shared" si="1"/>
         <v>2.0299475</v>
       </c>
-      <c r="K74" s="61"/>
+      <c r="K74" s="61">
+        <v>45105</v>
+      </c>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
-      <c r="N74" s="58"/>
-      <c r="O74" s="58"/>
-      <c r="P74" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q74" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R74" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S74" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T74" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U74" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N74" s="177">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="O74" s="177" t="s">
+        <v>411</v>
+      </c>
+      <c r="P74" s="177">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="Q74" s="177">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="R74" s="178" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="S74" s="177">
+        <v>344</v>
+      </c>
+      <c r="T74" s="177">
+        <v>0.249</v>
+      </c>
+      <c r="U74" s="178" t="e">
+        <v>#VALUE!</v>
       </c>
       <c r="V74" s="1"/>
       <c r="W74" s="1"/>
@@ -6386,8 +6392,8 @@
       <c r="E75" s="59">
         <v>1</v>
       </c>
-      <c r="F75" s="132" t="s">
-        <v>394</v>
+      <c r="F75" s="173">
+        <v>44761</v>
       </c>
       <c r="G75" s="60">
         <v>2.0744600000000002</v>
@@ -6403,34 +6409,34 @@
         <f t="shared" si="1"/>
         <v>2.0230874999999999</v>
       </c>
-      <c r="K75" s="61"/>
+      <c r="K75" s="61">
+        <v>45105</v>
+      </c>
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
-      <c r="N75" s="58"/>
-      <c r="O75" s="58"/>
-      <c r="P75" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q75" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R75" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S75" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T75" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U75" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N75" s="177">
+        <v>0.78</v>
+      </c>
+      <c r="O75" s="177">
+        <v>1.556</v>
+      </c>
+      <c r="P75" s="177">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="Q75" s="177">
+        <v>0.375</v>
+      </c>
+      <c r="R75" s="177">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="S75" s="177">
+        <v>344</v>
+      </c>
+      <c r="T75" s="177">
+        <v>0.32</v>
+      </c>
+      <c r="U75" s="177">
+        <v>2.775048768E-3</v>
       </c>
       <c r="V75" s="1"/>
       <c r="W75" s="1"/>
@@ -6452,8 +6458,8 @@
       <c r="E76" s="59">
         <v>1</v>
       </c>
-      <c r="F76" s="133" t="s">
-        <v>394</v>
+      <c r="F76" s="173">
+        <v>44761</v>
       </c>
       <c r="G76" s="60">
         <v>2.0345599999999999</v>
@@ -6469,34 +6475,34 @@
         <f t="shared" si="1"/>
         <v>2.0912875</v>
       </c>
-      <c r="K76" s="61"/>
+      <c r="K76" s="61">
+        <v>45105</v>
+      </c>
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
-      <c r="N76" s="58"/>
-      <c r="O76" s="58"/>
-      <c r="P76" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q76" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R76" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S76" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T76" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U76" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N76" s="177">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="O76" s="177">
+        <v>1.6639999999999999</v>
+      </c>
+      <c r="P76" s="177">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="Q76" s="177">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="R76" s="177">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="S76" s="177">
+        <v>344</v>
+      </c>
+      <c r="T76" s="177">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="U76" s="177">
+        <v>2.3404909699999998E-3</v>
       </c>
       <c r="V76" s="1"/>
       <c r="W76" s="1"/>
@@ -6518,8 +6524,8 @@
       <c r="E77" s="59">
         <v>1</v>
       </c>
-      <c r="F77" s="132" t="s">
-        <v>394</v>
+      <c r="F77" s="173">
+        <v>44761</v>
       </c>
       <c r="G77" s="60">
         <v>2.09768</v>
@@ -6535,34 +6541,34 @@
         <f t="shared" si="1"/>
         <v>2.0233875000000001</v>
       </c>
-      <c r="K77" s="61"/>
+      <c r="K77" s="61">
+        <v>45105</v>
+      </c>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
-      <c r="N77" s="58"/>
-      <c r="O77" s="58"/>
-      <c r="P77" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q77" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R77" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S77" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T77" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U77" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N77" s="177">
+        <v>0.747</v>
+      </c>
+      <c r="O77" s="177">
+        <v>1.5960000000000001</v>
+      </c>
+      <c r="P77" s="177">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="Q77" s="177">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="R77" s="177">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="S77" s="177">
+        <v>344</v>
+      </c>
+      <c r="T77" s="177">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="U77" s="177">
+        <v>2.2620884309999998E-3</v>
       </c>
       <c r="V77" s="1"/>
       <c r="W77" s="1"/>
@@ -6584,8 +6590,8 @@
       <c r="E78" s="59">
         <v>1</v>
       </c>
-      <c r="F78" s="133" t="s">
-        <v>394</v>
+      <c r="F78" s="173">
+        <v>44761</v>
       </c>
       <c r="G78" s="60">
         <v>2.0266199999999999</v>
@@ -6601,34 +6607,34 @@
         <f t="shared" si="1"/>
         <v>2.0697274999999999</v>
       </c>
-      <c r="K78" s="61"/>
+      <c r="K78" s="61">
+        <v>45105</v>
+      </c>
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
-      <c r="N78" s="58"/>
-      <c r="O78" s="58"/>
-      <c r="P78" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q78" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R78" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S78" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T78" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U78" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N78" s="177">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="O78" s="177">
+        <v>1.7010000000000001</v>
+      </c>
+      <c r="P78" s="177">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="Q78" s="177">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="R78" s="177">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="S78" s="177">
+        <v>344</v>
+      </c>
+      <c r="T78" s="177">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="U78" s="177">
+        <v>1.8168674170000001E-3</v>
       </c>
       <c r="V78" s="1"/>
       <c r="W78" s="1"/>
@@ -6650,8 +6656,8 @@
       <c r="E79" s="59">
         <v>1</v>
       </c>
-      <c r="F79" s="132" t="s">
-        <v>395</v>
+      <c r="F79" s="173">
+        <v>44763</v>
       </c>
       <c r="G79" s="60">
         <v>2.0036</v>
@@ -6667,34 +6673,34 @@
         <f t="shared" si="1"/>
         <v>2.0575775000000003</v>
       </c>
-      <c r="K79" s="61"/>
+      <c r="K79" s="61">
+        <v>45106</v>
+      </c>
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
-      <c r="N79" s="58"/>
-      <c r="O79" s="58"/>
-      <c r="P79" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q79" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R79" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S79" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T79" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U79" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N79" s="177" t="s">
+        <v>411</v>
+      </c>
+      <c r="O79" s="177">
+        <v>1.6120000000000001</v>
+      </c>
+      <c r="P79" s="178" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q79" s="178" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R79" s="177">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="S79" s="177">
+        <v>343</v>
+      </c>
+      <c r="T79" s="178" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="U79" s="178" t="e">
+        <v>#VALUE!</v>
       </c>
       <c r="V79" s="1"/>
       <c r="W79" s="1"/>
@@ -6716,8 +6722,8 @@
       <c r="E80" s="59">
         <v>1</v>
       </c>
-      <c r="F80" s="133" t="s">
-        <v>395</v>
+      <c r="F80" s="173">
+        <v>44763</v>
       </c>
       <c r="G80" s="60">
         <v>2.0432000000000001</v>
@@ -6733,34 +6739,34 @@
         <f t="shared" si="1"/>
         <v>1.9799074999999999</v>
       </c>
-      <c r="K80" s="61"/>
+      <c r="K80" s="61">
+        <v>45106</v>
+      </c>
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
-      <c r="N80" s="58"/>
-      <c r="O80" s="58"/>
-      <c r="P80" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q80" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R80" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S80" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T80" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U80" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N80" s="177">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="O80" s="177">
+        <v>1.532</v>
+      </c>
+      <c r="P80" s="177">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="Q80" s="177">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="R80" s="177">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="S80" s="177">
+        <v>343</v>
+      </c>
+      <c r="T80" s="177">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="U80" s="177">
+        <v>3.0189019510000002E-3</v>
       </c>
       <c r="V80" s="1"/>
       <c r="W80" s="1"/>
@@ -6782,8 +6788,8 @@
       <c r="E81" s="59">
         <v>1</v>
       </c>
-      <c r="F81" s="132" t="s">
-        <v>395</v>
+      <c r="F81" s="173">
+        <v>44763</v>
       </c>
       <c r="G81" s="60">
         <v>2.1815500000000001</v>
@@ -6799,34 +6805,34 @@
         <f t="shared" si="1"/>
         <v>1.9690875000000001</v>
       </c>
-      <c r="K81" s="61"/>
+      <c r="K81" s="61">
+        <v>45106</v>
+      </c>
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
-      <c r="N81" s="58"/>
-      <c r="O81" s="58"/>
-      <c r="P81" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q81" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R81" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S81" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T81" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U81" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N81" s="177">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="O81" s="177">
+        <v>1.645</v>
+      </c>
+      <c r="P81" s="177">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="Q81" s="177">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="R81" s="177">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="S81" s="177">
+        <v>343</v>
+      </c>
+      <c r="T81" s="177">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="U81" s="177">
+        <v>1.838416826E-3</v>
       </c>
       <c r="V81" s="1"/>
       <c r="W81" s="1"/>
@@ -6848,8 +6854,8 @@
       <c r="E82" s="59">
         <v>1</v>
       </c>
-      <c r="F82" s="133" t="s">
-        <v>395</v>
+      <c r="F82" s="173">
+        <v>44763</v>
       </c>
       <c r="G82" s="60">
         <v>2.02542</v>
@@ -6865,34 +6871,34 @@
         <f t="shared" si="1"/>
         <v>2.0169174999999999</v>
       </c>
-      <c r="K82" s="61"/>
+      <c r="K82" s="61">
+        <v>45106</v>
+      </c>
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
-      <c r="N82" s="58"/>
-      <c r="O82" s="58"/>
-      <c r="P82" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q82" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R82" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S82" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T82" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U82" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N82" s="177">
+        <v>1.012</v>
+      </c>
+      <c r="O82" s="177">
+        <v>1.6220000000000001</v>
+      </c>
+      <c r="P82" s="177">
+        <v>0.43</v>
+      </c>
+      <c r="Q82" s="177">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="R82" s="177">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="S82" s="177">
+        <v>343</v>
+      </c>
+      <c r="T82" s="177">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="U82" s="177">
+        <v>3.4553646650000002E-3</v>
       </c>
       <c r="V82" s="1"/>
       <c r="W82" s="1"/>
@@ -6914,8 +6920,8 @@
       <c r="E83" s="59">
         <v>1</v>
       </c>
-      <c r="F83" s="132" t="s">
-        <v>395</v>
+      <c r="F83" s="173">
+        <v>44763</v>
       </c>
       <c r="G83" s="60">
         <v>2.1057600000000001</v>
@@ -6931,34 +6937,34 @@
         <f t="shared" si="1"/>
         <v>2.0142475000000002</v>
       </c>
-      <c r="K83" s="61"/>
+      <c r="K83" s="61">
+        <v>45106</v>
+      </c>
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
-      <c r="N83" s="58"/>
-      <c r="O83" s="58"/>
-      <c r="P83" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q83" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R83" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S83" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T83" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U83" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N83" s="177">
+        <v>0.874</v>
+      </c>
+      <c r="O83" s="177">
+        <v>1.581</v>
+      </c>
+      <c r="P83" s="177">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="Q83" s="177">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="R83" s="177">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="S83" s="177">
+        <v>343</v>
+      </c>
+      <c r="T83" s="177">
+        <v>0.372</v>
+      </c>
+      <c r="U83" s="177">
+        <v>2.821044328E-3</v>
       </c>
       <c r="V83" s="1"/>
       <c r="W83" s="1"/>
@@ -6980,8 +6986,8 @@
       <c r="E84" s="59">
         <v>1</v>
       </c>
-      <c r="F84" s="133" t="s">
-        <v>395</v>
+      <c r="F84" s="173">
+        <v>44763</v>
       </c>
       <c r="G84" s="60">
         <v>2.0706799999999999</v>
@@ -6997,34 +7003,34 @@
         <f t="shared" si="1"/>
         <v>2.0573075000000003</v>
       </c>
-      <c r="K84" s="61"/>
+      <c r="K84" s="61">
+        <v>45106</v>
+      </c>
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
-      <c r="N84" s="58"/>
-      <c r="O84" s="58"/>
-      <c r="P84" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q84" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R84" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S84" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T84" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U84" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N84" s="177">
+        <v>0.752</v>
+      </c>
+      <c r="O84" s="177">
+        <v>1.7070000000000001</v>
+      </c>
+      <c r="P84" s="177">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="Q84" s="177">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="R84" s="177">
+        <v>0.83</v>
+      </c>
+      <c r="S84" s="177">
+        <v>343</v>
+      </c>
+      <c r="T84" s="177">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="U84" s="177">
+        <v>1.702975232E-3</v>
       </c>
       <c r="V84" s="1"/>
       <c r="W84" s="1"/>
@@ -7046,8 +7052,8 @@
       <c r="E85" s="59">
         <v>1</v>
       </c>
-      <c r="F85" s="132" t="s">
-        <v>395</v>
+      <c r="F85" s="173">
+        <v>44763</v>
       </c>
       <c r="G85" s="60">
         <v>2.1566100000000001</v>
@@ -7063,34 +7069,34 @@
         <f t="shared" si="1"/>
         <v>2.1296075000000001</v>
       </c>
-      <c r="K85" s="61"/>
+      <c r="K85" s="61">
+        <v>45106</v>
+      </c>
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
-      <c r="N85" s="58"/>
-      <c r="O85" s="58"/>
-      <c r="P85" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q85" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R85" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S85" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T85" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U85" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N85" s="177">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="O85" s="177">
+        <v>1.6319999999999999</v>
+      </c>
+      <c r="P85" s="177">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="Q85" s="177">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="R85" s="177">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="S85" s="177">
+        <v>343</v>
+      </c>
+      <c r="T85" s="177">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="U85" s="177">
+        <v>2.3864563549999998E-3</v>
       </c>
       <c r="V85" s="1"/>
       <c r="W85" s="1"/>
@@ -7112,8 +7118,8 @@
       <c r="E86" s="59">
         <v>1</v>
       </c>
-      <c r="F86" s="133" t="s">
-        <v>395</v>
+      <c r="F86" s="173">
+        <v>44763</v>
       </c>
       <c r="G86" s="60">
         <v>2.1099800000000002</v>
@@ -7129,34 +7135,34 @@
         <f t="shared" si="1"/>
         <v>2.0779274999999999</v>
       </c>
-      <c r="K86" s="61"/>
+      <c r="K86" s="61">
+        <v>45106</v>
+      </c>
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
-      <c r="N86" s="58"/>
-      <c r="O86" s="58"/>
-      <c r="P86" s="58">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q86" s="58">
-        <f t="shared" si="3"/>
-        <v>0.65558194774346801</v>
-      </c>
-      <c r="R86" s="58">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S86" s="58" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T86" s="58">
-        <f t="shared" si="6"/>
-        <v>-0.18764845605700708</v>
-      </c>
-      <c r="U86" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#NUM!</v>
+      <c r="N86" s="177">
+        <v>0.753</v>
+      </c>
+      <c r="O86" s="177">
+        <v>1.605</v>
+      </c>
+      <c r="P86" s="177">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="Q86" s="177">
+        <v>0.39</v>
+      </c>
+      <c r="R86" s="177">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="S86" s="177">
+        <v>343</v>
+      </c>
+      <c r="T86" s="177">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="U86" s="177">
+        <v>2.5514808530000001E-3</v>
       </c>
       <c r="V86" s="1"/>
       <c r="W86" s="1"/>
@@ -7174,7 +7180,7 @@
         <v>117</v>
       </c>
       <c r="E87" s="59"/>
-      <c r="F87" s="132"/>
+      <c r="F87" s="174"/>
       <c r="G87" s="60">
         <v>2.0176400000000001</v>
       </c>
@@ -7234,7 +7240,7 @@
         <v>117</v>
       </c>
       <c r="E88" s="59"/>
-      <c r="F88" s="134"/>
+      <c r="F88" s="175"/>
       <c r="G88" s="3">
         <v>1.9499500000000001</v>
       </c>
@@ -7294,6 +7300,7 @@
         <v>117</v>
       </c>
       <c r="E89" s="59"/>
+      <c r="F89" s="176"/>
       <c r="G89" s="3">
         <v>2.1017299999999999</v>
       </c>
@@ -7353,6 +7360,7 @@
         <v>117</v>
       </c>
       <c r="E90" s="59"/>
+      <c r="F90" s="176"/>
       <c r="G90" s="3">
         <v>2.11707</v>
       </c>
@@ -7412,6 +7420,7 @@
         <v>117</v>
       </c>
       <c r="E91" s="59"/>
+      <c r="F91" s="176"/>
       <c r="G91" s="3">
         <v>2.0811000000000002</v>
       </c>
@@ -7471,6 +7480,7 @@
         <v>117</v>
       </c>
       <c r="E92" s="59"/>
+      <c r="F92" s="176"/>
       <c r="G92" s="3">
         <v>2.0568599999999999</v>
       </c>
@@ -8226,17 +8236,17 @@
     </row>
     <row r="105" spans="1:26" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
-      <c r="B105" s="173" t="s">
+      <c r="B105" s="132" t="s">
+        <v>393</v>
+      </c>
+      <c r="C105" s="132" t="s">
+        <v>394</v>
+      </c>
+      <c r="D105" s="132" t="s">
+        <v>395</v>
+      </c>
+      <c r="E105" s="132" t="s">
         <v>396</v>
-      </c>
-      <c r="C105" s="173" t="s">
-        <v>397</v>
-      </c>
-      <c r="D105" s="173" t="s">
-        <v>398</v>
-      </c>
-      <c r="E105" s="173" t="s">
-        <v>399</v>
       </c>
       <c r="F105" s="62"/>
       <c r="G105" s="1"/>
@@ -8286,16 +8296,16 @@
     </row>
     <row r="106" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
-      <c r="B106" s="174" t="s">
-        <v>400</v>
-      </c>
-      <c r="C106" s="175">
+      <c r="B106" s="133" t="s">
+        <v>397</v>
+      </c>
+      <c r="C106" s="134">
         <v>45122</v>
       </c>
-      <c r="D106" s="174" t="s">
-        <v>401</v>
-      </c>
-      <c r="E106" s="174">
+      <c r="D106" s="133" t="s">
+        <v>398</v>
+      </c>
+      <c r="E106" s="133">
         <v>0.76100000000000001</v>
       </c>
       <c r="F106" s="62"/>
@@ -8346,16 +8356,16 @@
     </row>
     <row r="107" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
-      <c r="B107" s="174" t="s">
-        <v>402</v>
-      </c>
-      <c r="C107" s="175">
+      <c r="B107" s="133" t="s">
+        <v>399</v>
+      </c>
+      <c r="C107" s="134">
         <v>45122</v>
       </c>
-      <c r="D107" s="174" t="s">
-        <v>403</v>
-      </c>
-      <c r="E107" s="174">
+      <c r="D107" s="133" t="s">
+        <v>400</v>
+      </c>
+      <c r="E107" s="133">
         <v>2.6259999999999999</v>
       </c>
       <c r="F107" s="62"/>
@@ -8406,16 +8416,16 @@
     </row>
     <row r="108" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
-      <c r="B108" s="174" t="s">
-        <v>402</v>
-      </c>
-      <c r="C108" s="175">
+      <c r="B108" s="133" t="s">
+        <v>399</v>
+      </c>
+      <c r="C108" s="134">
         <v>45122</v>
       </c>
-      <c r="D108" s="174" t="s">
-        <v>404</v>
-      </c>
-      <c r="E108" s="174">
+      <c r="D108" s="133" t="s">
+        <v>401</v>
+      </c>
+      <c r="E108" s="133">
         <v>3.4350000000000001</v>
       </c>
       <c r="F108" s="62"/>
@@ -8466,16 +8476,16 @@
     </row>
     <row r="109" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
-      <c r="B109" s="174" t="s">
-        <v>405</v>
-      </c>
-      <c r="C109" s="175">
+      <c r="B109" s="133" t="s">
+        <v>402</v>
+      </c>
+      <c r="C109" s="134">
         <v>45122</v>
       </c>
-      <c r="D109" s="174" t="s">
-        <v>403</v>
-      </c>
-      <c r="E109" s="174">
+      <c r="D109" s="133" t="s">
+        <v>400</v>
+      </c>
+      <c r="E109" s="133">
         <v>0.94099999999999995</v>
       </c>
       <c r="F109" s="62"/>
@@ -8526,16 +8536,16 @@
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
-      <c r="B110" s="174" t="s">
-        <v>405</v>
-      </c>
-      <c r="C110" s="175">
+      <c r="B110" s="133" t="s">
+        <v>402</v>
+      </c>
+      <c r="C110" s="134">
         <v>45122</v>
       </c>
-      <c r="D110" s="174" t="s">
-        <v>404</v>
-      </c>
-      <c r="E110" s="174">
+      <c r="D110" s="133" t="s">
+        <v>401</v>
+      </c>
+      <c r="E110" s="133">
         <v>1.623</v>
       </c>
       <c r="F110" s="62"/>
@@ -8586,16 +8596,16 @@
     </row>
     <row r="111" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
-      <c r="B111" s="174" t="s">
-        <v>406</v>
-      </c>
-      <c r="C111" s="175">
+      <c r="B111" s="133" t="s">
+        <v>403</v>
+      </c>
+      <c r="C111" s="134">
         <v>45123</v>
       </c>
-      <c r="D111" s="174" t="s">
-        <v>403</v>
-      </c>
-      <c r="E111" s="174">
+      <c r="D111" s="133" t="s">
+        <v>400</v>
+      </c>
+      <c r="E111" s="133">
         <v>0.98699999999999999</v>
       </c>
       <c r="F111" s="62"/>
@@ -8646,16 +8656,16 @@
     </row>
     <row r="112" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
-      <c r="B112" s="174" t="s">
-        <v>406</v>
-      </c>
-      <c r="C112" s="175">
+      <c r="B112" s="133" t="s">
+        <v>403</v>
+      </c>
+      <c r="C112" s="134">
         <v>45123</v>
       </c>
-      <c r="D112" s="174" t="s">
-        <v>404</v>
-      </c>
-      <c r="E112" s="174">
+      <c r="D112" s="133" t="s">
+        <v>401</v>
+      </c>
+      <c r="E112" s="133">
         <v>1.5169999999999999</v>
       </c>
       <c r="F112" s="62"/>
@@ -8706,16 +8716,16 @@
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
-      <c r="B113" s="174" t="s">
-        <v>407</v>
-      </c>
-      <c r="C113" s="175">
+      <c r="B113" s="133" t="s">
+        <v>404</v>
+      </c>
+      <c r="C113" s="134">
         <v>45136</v>
       </c>
-      <c r="D113" s="174" t="s">
-        <v>403</v>
-      </c>
-      <c r="E113" s="174">
+      <c r="D113" s="133" t="s">
+        <v>400</v>
+      </c>
+      <c r="E113" s="133">
         <v>0.93899999999999995</v>
       </c>
       <c r="F113" s="62"/>
@@ -8766,16 +8776,16 @@
     </row>
     <row r="114" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
-      <c r="B114" s="174" t="s">
-        <v>407</v>
-      </c>
-      <c r="C114" s="175">
+      <c r="B114" s="133" t="s">
+        <v>404</v>
+      </c>
+      <c r="C114" s="134">
         <v>45136</v>
       </c>
-      <c r="D114" s="174" t="s">
-        <v>404</v>
-      </c>
-      <c r="E114" s="174">
+      <c r="D114" s="133" t="s">
+        <v>401</v>
+      </c>
+      <c r="E114" s="133">
         <v>1.6040000000000001</v>
       </c>
       <c r="F114" s="62"/>
@@ -8826,16 +8836,16 @@
     </row>
     <row r="115" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
-      <c r="B115" s="174" t="s">
-        <v>408</v>
-      </c>
-      <c r="C115" s="175">
+      <c r="B115" s="133" t="s">
+        <v>405</v>
+      </c>
+      <c r="C115" s="134">
         <v>45136</v>
       </c>
-      <c r="D115" s="174" t="s">
-        <v>404</v>
-      </c>
-      <c r="E115" s="174">
+      <c r="D115" s="133" t="s">
+        <v>401</v>
+      </c>
+      <c r="E115" s="133">
         <v>1.37</v>
       </c>
       <c r="F115" s="62"/>
@@ -8886,16 +8896,16 @@
     </row>
     <row r="116" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
-      <c r="B116" s="174" t="s">
-        <v>409</v>
-      </c>
-      <c r="C116" s="175">
+      <c r="B116" s="133" t="s">
+        <v>406</v>
+      </c>
+      <c r="C116" s="134">
         <v>45136</v>
       </c>
-      <c r="D116" s="174" t="s">
-        <v>403</v>
-      </c>
-      <c r="E116" s="174">
+      <c r="D116" s="133" t="s">
+        <v>400</v>
+      </c>
+      <c r="E116" s="133">
         <v>0.65900000000000003</v>
       </c>
       <c r="F116" s="62"/>
@@ -8946,16 +8956,16 @@
     </row>
     <row r="117" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
-      <c r="B117" s="174" t="s">
-        <v>409</v>
-      </c>
-      <c r="C117" s="175">
+      <c r="B117" s="133" t="s">
+        <v>406</v>
+      </c>
+      <c r="C117" s="134">
         <v>45136</v>
       </c>
-      <c r="D117" s="174" t="s">
-        <v>404</v>
-      </c>
-      <c r="E117" s="174">
+      <c r="D117" s="133" t="s">
+        <v>401</v>
+      </c>
+      <c r="E117" s="133">
         <v>1.675</v>
       </c>
       <c r="F117" s="62"/>
@@ -9006,16 +9016,16 @@
     </row>
     <row r="118" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
-      <c r="B118" s="174" t="s">
-        <v>410</v>
-      </c>
-      <c r="C118" s="174" t="s">
-        <v>411</v>
-      </c>
-      <c r="D118" s="174" t="s">
-        <v>403</v>
-      </c>
-      <c r="E118" s="174">
+      <c r="B118" s="133" t="s">
+        <v>407</v>
+      </c>
+      <c r="C118" s="133" t="s">
+        <v>408</v>
+      </c>
+      <c r="D118" s="133" t="s">
+        <v>400</v>
+      </c>
+      <c r="E118" s="133">
         <v>0.70299999999999996</v>
       </c>
       <c r="F118" s="62"/>
@@ -9066,16 +9076,16 @@
     </row>
     <row r="119" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
-      <c r="B119" s="174" t="s">
-        <v>410</v>
-      </c>
-      <c r="C119" s="174" t="s">
-        <v>411</v>
-      </c>
-      <c r="D119" s="174" t="s">
-        <v>404</v>
-      </c>
-      <c r="E119" s="174">
+      <c r="B119" s="133" t="s">
+        <v>407</v>
+      </c>
+      <c r="C119" s="133" t="s">
+        <v>408</v>
+      </c>
+      <c r="D119" s="133" t="s">
+        <v>401</v>
+      </c>
+      <c r="E119" s="133">
         <v>1.5820000000000001</v>
       </c>
       <c r="F119" s="62"/>
@@ -9126,16 +9136,16 @@
     </row>
     <row r="120" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
-      <c r="B120" s="174" t="s">
-        <v>412</v>
-      </c>
-      <c r="C120" s="174" t="s">
-        <v>411</v>
-      </c>
-      <c r="D120" s="174" t="s">
-        <v>403</v>
-      </c>
-      <c r="E120" s="174">
+      <c r="B120" s="133" t="s">
+        <v>409</v>
+      </c>
+      <c r="C120" s="133" t="s">
+        <v>408</v>
+      </c>
+      <c r="D120" s="133" t="s">
+        <v>400</v>
+      </c>
+      <c r="E120" s="133">
         <v>0.88900000000000001</v>
       </c>
       <c r="F120" s="62"/>
@@ -9186,16 +9196,16 @@
     </row>
     <row r="121" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
-      <c r="B121" s="174" t="s">
-        <v>412</v>
-      </c>
-      <c r="C121" s="174" t="s">
-        <v>411</v>
-      </c>
-      <c r="D121" s="174" t="s">
-        <v>404</v>
-      </c>
-      <c r="E121" s="174">
+      <c r="B121" s="133" t="s">
+        <v>409</v>
+      </c>
+      <c r="C121" s="133" t="s">
+        <v>408</v>
+      </c>
+      <c r="D121" s="133" t="s">
+        <v>401</v>
+      </c>
+      <c r="E121" s="133">
         <v>1.6</v>
       </c>
       <c r="F121" s="62"/>
@@ -9246,16 +9256,16 @@
     </row>
     <row r="122" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
-      <c r="B122" s="174" t="s">
-        <v>413</v>
-      </c>
-      <c r="C122" s="174" t="s">
-        <v>411</v>
-      </c>
-      <c r="D122" s="174" t="s">
-        <v>403</v>
-      </c>
-      <c r="E122" s="174">
+      <c r="B122" s="133" t="s">
+        <v>410</v>
+      </c>
+      <c r="C122" s="133" t="s">
+        <v>408</v>
+      </c>
+      <c r="D122" s="133" t="s">
+        <v>400</v>
+      </c>
+      <c r="E122" s="133">
         <v>0.69799999999999995</v>
       </c>
       <c r="F122" s="62"/>
@@ -9306,16 +9316,16 @@
     </row>
     <row r="123" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
-      <c r="B123" s="174" t="s">
-        <v>413</v>
-      </c>
-      <c r="C123" s="174" t="s">
-        <v>411</v>
-      </c>
-      <c r="D123" s="174" t="s">
-        <v>404</v>
-      </c>
-      <c r="E123" s="174">
+      <c r="B123" s="133" t="s">
+        <v>410</v>
+      </c>
+      <c r="C123" s="133" t="s">
+        <v>408</v>
+      </c>
+      <c r="D123" s="133" t="s">
+        <v>401</v>
+      </c>
+      <c r="E123" s="133">
         <v>1.538</v>
       </c>
       <c r="F123" s="62"/>
@@ -35342,32 +35352,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="M39:T39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:F43"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="E44:F44"/>
     <mergeCell ref="B51:E51"/>
@@ -35382,8 +35366,34 @@
     <mergeCell ref="B47:D47"/>
     <mergeCell ref="E47:F47"/>
     <mergeCell ref="F51:K51"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="M39:T39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
   </mergeCells>
-  <conditionalFormatting sqref="N59:U184">
+  <conditionalFormatting sqref="N59:U62 N87:U184">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>ISERROR(N59)</formula>
     </cfRule>
@@ -35430,7 +35440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
+    <sheetView topLeftCell="A63" workbookViewId="0">
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
@@ -41365,7 +41375,7 @@
       </c>
       <c r="D7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>3039</v>
+        <v>3061</v>
       </c>
       <c r="E7" s="117" t="s">
         <v>298</v>
@@ -41415,7 +41425,7 @@
       </c>
       <c r="D9" s="122">
         <f t="shared" ref="D9:D12" ca="1" si="1">IF(AND(C9&lt;&gt;"",B9&lt;&gt;"Resolved"),TODAY()-C9,"")</f>
-        <v>3039</v>
+        <v>3061</v>
       </c>
       <c r="E9" s="122" t="s">
         <v>298</v>

</xml_diff>

<commit_message>
Edited ANOVAs for teabag analysis
</commit_message>
<xml_diff>
--- a/Tea_bag_analysis/Tea_bag_decomposition_non-woven.xlsx
+++ b/Tea_bag_analysis/Tea_bag_decomposition_non-woven.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfilewych1/Documents/GitHub/Garibaldi/Tea_bag_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35FFA52-9202-3046-B489-136874E24272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9458FCE-8F59-3B49-B9E3-4F72C80D127B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="760" windowWidth="29780" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6140" yWindow="1260" windowWidth="33720" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -3092,68 +3092,32 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3162,12 +3126,48 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3441,8 +3441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="V61" sqref="V61"/>
+    <sheetView topLeftCell="G54" workbookViewId="0">
+      <selection activeCell="U60" sqref="U60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3802,12 +3802,12 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
-      <c r="B12" s="135" t="s">
+      <c r="B12" s="178" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="136"/>
-      <c r="D12" s="136"/>
-      <c r="E12" s="136"/>
+      <c r="C12" s="147"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="147"/>
       <c r="F12" s="14"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
@@ -3832,12 +3832,12 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
-      <c r="B13" s="137" t="s">
+      <c r="B13" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="138"/>
-      <c r="D13" s="138"/>
-      <c r="E13" s="138"/>
+      <c r="C13" s="174"/>
+      <c r="D13" s="174"/>
+      <c r="E13" s="174"/>
       <c r="F13" s="17"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
@@ -3862,12 +3862,12 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
-      <c r="B14" s="137" t="s">
+      <c r="B14" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="138"/>
-      <c r="D14" s="138"/>
-      <c r="E14" s="138"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="174"/>
       <c r="F14" s="18"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -3892,12 +3892,12 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
-      <c r="B15" s="137" t="s">
+      <c r="B15" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="138"/>
+      <c r="C15" s="174"/>
+      <c r="D15" s="174"/>
+      <c r="E15" s="174"/>
       <c r="F15" s="18"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -3922,12 +3922,12 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
-      <c r="B16" s="137" t="s">
+      <c r="B16" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="138"/>
-      <c r="D16" s="138"/>
-      <c r="E16" s="138"/>
+      <c r="C16" s="174"/>
+      <c r="D16" s="174"/>
+      <c r="E16" s="174"/>
       <c r="F16" s="18"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -3952,12 +3952,12 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
-      <c r="B17" s="137" t="s">
+      <c r="B17" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="138"/>
-      <c r="D17" s="138"/>
-      <c r="E17" s="138"/>
+      <c r="C17" s="174"/>
+      <c r="D17" s="174"/>
+      <c r="E17" s="174"/>
       <c r="F17" s="18"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -3982,12 +3982,12 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
-      <c r="B18" s="137" t="s">
+      <c r="B18" s="173" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="138"/>
-      <c r="D18" s="138"/>
-      <c r="E18" s="138"/>
+      <c r="C18" s="174"/>
+      <c r="D18" s="174"/>
+      <c r="E18" s="174"/>
       <c r="F18" s="18"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -4012,12 +4012,12 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
-      <c r="B19" s="139" t="s">
+      <c r="B19" s="177" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="140"/>
-      <c r="D19" s="140"/>
-      <c r="E19" s="140"/>
+      <c r="C19" s="150"/>
+      <c r="D19" s="150"/>
+      <c r="E19" s="150"/>
       <c r="F19" s="20"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -4162,12 +4162,12 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
-      <c r="B24" s="135" t="s">
+      <c r="B24" s="178" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="136"/>
-      <c r="D24" s="136"/>
-      <c r="E24" s="136"/>
+      <c r="C24" s="147"/>
+      <c r="D24" s="147"/>
+      <c r="E24" s="147"/>
       <c r="F24" s="23">
         <v>0.84199999999999997</v>
       </c>
@@ -4194,12 +4194,12 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
-      <c r="B25" s="137" t="s">
+      <c r="B25" s="173" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="138"/>
-      <c r="D25" s="138"/>
-      <c r="E25" s="138"/>
+      <c r="C25" s="174"/>
+      <c r="D25" s="174"/>
+      <c r="E25" s="174"/>
       <c r="F25" s="24">
         <v>0.55200000000000005</v>
       </c>
@@ -4226,12 +4226,12 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
-      <c r="B26" s="137" t="s">
+      <c r="B26" s="173" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="138"/>
-      <c r="D26" s="138"/>
-      <c r="E26" s="138"/>
+      <c r="C26" s="174"/>
+      <c r="D26" s="174"/>
+      <c r="E26" s="174"/>
       <c r="F26" s="25">
         <v>0.2494625</v>
       </c>
@@ -4258,12 +4258,12 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
-      <c r="B27" s="137" t="s">
+      <c r="B27" s="173" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="138"/>
-      <c r="D27" s="138"/>
-      <c r="E27" s="138"/>
+      <c r="C27" s="174"/>
+      <c r="D27" s="174"/>
+      <c r="E27" s="174"/>
       <c r="F27" s="26"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -4318,12 +4318,12 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
-      <c r="B29" s="137" t="s">
+      <c r="B29" s="173" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="138"/>
-      <c r="D29" s="138"/>
-      <c r="E29" s="138"/>
+      <c r="C29" s="174"/>
+      <c r="D29" s="174"/>
+      <c r="E29" s="174"/>
       <c r="F29" s="26"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -4442,13 +4442,13 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
-      <c r="B33" s="141" t="s">
+      <c r="B33" s="175" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="142"/>
-      <c r="D33" s="142"/>
-      <c r="E33" s="142"/>
-      <c r="F33" s="143"/>
+      <c r="C33" s="169"/>
+      <c r="D33" s="169"/>
+      <c r="E33" s="169"/>
+      <c r="F33" s="170"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
@@ -4472,13 +4472,13 @@
     </row>
     <row r="34" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9"/>
-      <c r="B34" s="144" t="s">
+      <c r="B34" s="176" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="145"/>
-      <c r="D34" s="145"/>
-      <c r="E34" s="145"/>
-      <c r="F34" s="146"/>
+      <c r="C34" s="155"/>
+      <c r="D34" s="155"/>
+      <c r="E34" s="155"/>
+      <c r="F34" s="156"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
@@ -4620,16 +4620,16 @@
     </row>
     <row r="39" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
-      <c r="B39" s="147" t="s">
+      <c r="B39" s="167" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="140"/>
-      <c r="D39" s="140"/>
-      <c r="E39" s="148" t="s">
+      <c r="C39" s="150"/>
+      <c r="D39" s="150"/>
+      <c r="E39" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="F39" s="142"/>
-      <c r="G39" s="143"/>
+      <c r="F39" s="169"/>
+      <c r="G39" s="170"/>
       <c r="H39" s="30" t="s">
         <v>39</v>
       </c>
@@ -4637,16 +4637,16 @@
       <c r="J39" s="31"/>
       <c r="K39" s="31"/>
       <c r="L39" s="23"/>
-      <c r="M39" s="149" t="s">
+      <c r="M39" s="148" t="s">
         <v>40</v>
       </c>
-      <c r="N39" s="136"/>
-      <c r="O39" s="136"/>
-      <c r="P39" s="136"/>
-      <c r="Q39" s="136"/>
-      <c r="R39" s="136"/>
-      <c r="S39" s="136"/>
-      <c r="T39" s="150"/>
+      <c r="N39" s="147"/>
+      <c r="O39" s="147"/>
+      <c r="P39" s="147"/>
+      <c r="Q39" s="147"/>
+      <c r="R39" s="147"/>
+      <c r="S39" s="147"/>
+      <c r="T39" s="161"/>
       <c r="U39" s="9"/>
       <c r="V39" s="9"/>
       <c r="W39" s="9"/>
@@ -4656,15 +4656,15 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
-      <c r="B40" s="151" t="s">
+      <c r="B40" s="171" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="142"/>
-      <c r="D40" s="143"/>
-      <c r="E40" s="152" t="s">
+      <c r="C40" s="169"/>
+      <c r="D40" s="170"/>
+      <c r="E40" s="172" t="s">
         <v>42</v>
       </c>
-      <c r="F40" s="142"/>
+      <c r="F40" s="169"/>
       <c r="G40" s="33" t="s">
         <v>43</v>
       </c>
@@ -4716,13 +4716,13 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
-      <c r="B41" s="155" t="s">
+      <c r="B41" s="164" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="156"/>
-      <c r="D41" s="157"/>
-      <c r="E41" s="153"/>
-      <c r="F41" s="154"/>
+      <c r="C41" s="152"/>
+      <c r="D41" s="153"/>
+      <c r="E41" s="162"/>
+      <c r="F41" s="163"/>
       <c r="G41" s="37"/>
       <c r="H41" s="38"/>
       <c r="I41" s="39"/>
@@ -4746,13 +4746,13 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9"/>
-      <c r="B42" s="158" t="s">
+      <c r="B42" s="141" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="159"/>
-      <c r="D42" s="160"/>
-      <c r="E42" s="161"/>
-      <c r="F42" s="162"/>
+      <c r="C42" s="142"/>
+      <c r="D42" s="143"/>
+      <c r="E42" s="165"/>
+      <c r="F42" s="145"/>
       <c r="G42" s="41"/>
       <c r="H42" s="38"/>
       <c r="I42" s="39"/>
@@ -4776,11 +4776,11 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9"/>
-      <c r="B43" s="158"/>
-      <c r="C43" s="159"/>
-      <c r="D43" s="160"/>
-      <c r="E43" s="163"/>
-      <c r="F43" s="162"/>
+      <c r="B43" s="141"/>
+      <c r="C43" s="142"/>
+      <c r="D43" s="143"/>
+      <c r="E43" s="166"/>
+      <c r="F43" s="145"/>
       <c r="G43" s="41"/>
       <c r="H43" s="38"/>
       <c r="I43" s="39"/>
@@ -4804,11 +4804,11 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
-      <c r="B44" s="158"/>
-      <c r="C44" s="159"/>
-      <c r="D44" s="160"/>
-      <c r="E44" s="164"/>
-      <c r="F44" s="162"/>
+      <c r="B44" s="141"/>
+      <c r="C44" s="142"/>
+      <c r="D44" s="143"/>
+      <c r="E44" s="144"/>
+      <c r="F44" s="145"/>
       <c r="G44" s="18"/>
       <c r="H44" s="38"/>
       <c r="I44" s="39"/>
@@ -4832,11 +4832,11 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
-      <c r="B45" s="158"/>
-      <c r="C45" s="159"/>
-      <c r="D45" s="160"/>
-      <c r="E45" s="164"/>
-      <c r="F45" s="162"/>
+      <c r="B45" s="141"/>
+      <c r="C45" s="142"/>
+      <c r="D45" s="143"/>
+      <c r="E45" s="144"/>
+      <c r="F45" s="145"/>
       <c r="G45" s="18"/>
       <c r="H45" s="38"/>
       <c r="I45" s="39"/>
@@ -4860,11 +4860,11 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9"/>
-      <c r="B46" s="158"/>
-      <c r="C46" s="159"/>
-      <c r="D46" s="160"/>
-      <c r="E46" s="164"/>
-      <c r="F46" s="162"/>
+      <c r="B46" s="141"/>
+      <c r="C46" s="142"/>
+      <c r="D46" s="143"/>
+      <c r="E46" s="144"/>
+      <c r="F46" s="145"/>
       <c r="G46" s="18"/>
       <c r="H46" s="38"/>
       <c r="I46" s="39"/>
@@ -4888,11 +4888,11 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9"/>
-      <c r="B47" s="169"/>
-      <c r="C47" s="145"/>
-      <c r="D47" s="146"/>
-      <c r="E47" s="170"/>
-      <c r="F47" s="171"/>
+      <c r="B47" s="157"/>
+      <c r="C47" s="155"/>
+      <c r="D47" s="156"/>
+      <c r="E47" s="158"/>
+      <c r="F47" s="159"/>
       <c r="G47" s="20"/>
       <c r="H47" s="42"/>
       <c r="I47" s="43"/>
@@ -5004,20 +5004,20 @@
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
-      <c r="B51" s="165" t="s">
+      <c r="B51" s="146" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="136"/>
-      <c r="D51" s="136"/>
-      <c r="E51" s="136"/>
-      <c r="F51" s="172" t="s">
+      <c r="C51" s="147"/>
+      <c r="D51" s="147"/>
+      <c r="E51" s="147"/>
+      <c r="F51" s="160" t="s">
         <v>62</v>
       </c>
-      <c r="G51" s="136"/>
-      <c r="H51" s="136"/>
-      <c r="I51" s="136"/>
-      <c r="J51" s="136"/>
-      <c r="K51" s="150"/>
+      <c r="G51" s="147"/>
+      <c r="H51" s="147"/>
+      <c r="I51" s="147"/>
+      <c r="J51" s="147"/>
+      <c r="K51" s="161"/>
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
       <c r="N51" s="9"/>
@@ -5036,20 +5036,20 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9"/>
-      <c r="B52" s="149" t="s">
+      <c r="B52" s="148" t="s">
         <v>63</v>
       </c>
-      <c r="C52" s="136"/>
-      <c r="D52" s="136"/>
-      <c r="E52" s="136"/>
-      <c r="F52" s="167" t="s">
+      <c r="C52" s="147"/>
+      <c r="D52" s="147"/>
+      <c r="E52" s="147"/>
+      <c r="F52" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="G52" s="156"/>
-      <c r="H52" s="156"/>
-      <c r="I52" s="156"/>
-      <c r="J52" s="156"/>
-      <c r="K52" s="157"/>
+      <c r="G52" s="152"/>
+      <c r="H52" s="152"/>
+      <c r="I52" s="152"/>
+      <c r="J52" s="152"/>
+      <c r="K52" s="153"/>
       <c r="L52" s="9"/>
       <c r="M52" s="9"/>
       <c r="N52" s="9"/>
@@ -5068,20 +5068,20 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9"/>
-      <c r="B53" s="166" t="s">
+      <c r="B53" s="149" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="140"/>
-      <c r="D53" s="140"/>
-      <c r="E53" s="140"/>
-      <c r="F53" s="168" t="s">
+      <c r="C53" s="150"/>
+      <c r="D53" s="150"/>
+      <c r="E53" s="150"/>
+      <c r="F53" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="G53" s="145"/>
-      <c r="H53" s="145"/>
-      <c r="I53" s="145"/>
-      <c r="J53" s="145"/>
-      <c r="K53" s="146"/>
+      <c r="G53" s="155"/>
+      <c r="H53" s="155"/>
+      <c r="I53" s="155"/>
+      <c r="J53" s="155"/>
+      <c r="K53" s="156"/>
       <c r="L53" s="9"/>
       <c r="M53" s="9"/>
       <c r="N53" s="9"/>
@@ -5600,7 +5600,7 @@
       <c r="E63" s="59">
         <v>1</v>
       </c>
-      <c r="F63" s="173">
+      <c r="F63" s="135">
         <v>44762</v>
       </c>
       <c r="G63" s="60">
@@ -5622,28 +5622,28 @@
       </c>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
-      <c r="N63" s="177">
+      <c r="N63" s="139">
         <v>0.70899999999999996</v>
       </c>
-      <c r="O63" s="177">
+      <c r="O63" s="139">
         <v>1.694</v>
       </c>
-      <c r="P63" s="177">
+      <c r="P63" s="139">
         <v>0.61299999999999999</v>
       </c>
-      <c r="Q63" s="177">
+      <c r="Q63" s="139">
         <v>0.40200000000000002</v>
       </c>
-      <c r="R63" s="177">
+      <c r="R63" s="139">
         <v>0.85599999999999998</v>
       </c>
-      <c r="S63" s="177">
+      <c r="S63" s="139">
         <v>343</v>
       </c>
-      <c r="T63" s="177">
+      <c r="T63" s="139">
         <v>0.27300000000000002</v>
       </c>
-      <c r="U63" s="177">
+      <c r="U63" s="139">
         <v>1.298408996E-3</v>
       </c>
       <c r="V63" s="1"/>
@@ -5666,7 +5666,7 @@
       <c r="E64" s="59">
         <v>1</v>
       </c>
-      <c r="F64" s="173">
+      <c r="F64" s="135">
         <v>44762</v>
       </c>
       <c r="G64" s="60">
@@ -5688,28 +5688,28 @@
       </c>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
-      <c r="N64" s="177">
+      <c r="N64" s="139">
         <v>0.81699999999999995</v>
       </c>
-      <c r="O64" s="177">
+      <c r="O64" s="139">
         <v>1.643</v>
       </c>
-      <c r="P64" s="177">
+      <c r="P64" s="139">
         <v>0.55700000000000005</v>
       </c>
-      <c r="Q64" s="177">
+      <c r="Q64" s="139">
         <v>0.36499999999999999</v>
       </c>
-      <c r="R64" s="177">
+      <c r="R64" s="139">
         <v>0.77300000000000002</v>
       </c>
-      <c r="S64" s="177">
+      <c r="S64" s="139">
         <v>343</v>
       </c>
-      <c r="T64" s="177">
+      <c r="T64" s="139">
         <v>0.33800000000000002</v>
       </c>
-      <c r="U64" s="177">
+      <c r="U64" s="139">
         <v>2.835042937E-3</v>
       </c>
       <c r="V64" s="1"/>
@@ -5732,7 +5732,7 @@
       <c r="E65" s="59">
         <v>1</v>
       </c>
-      <c r="F65" s="173">
+      <c r="F65" s="135">
         <v>44762</v>
       </c>
       <c r="G65" s="60">
@@ -5754,28 +5754,28 @@
       </c>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
-      <c r="N65" s="177" t="s">
+      <c r="N65" s="139" t="s">
         <v>411</v>
       </c>
-      <c r="O65" s="177">
+      <c r="O65" s="139">
         <v>1.68</v>
       </c>
-      <c r="P65" s="178" t="e">
+      <c r="P65" s="140" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="Q65" s="178" t="e">
+      <c r="Q65" s="140" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="R65" s="177">
+      <c r="R65" s="139">
         <v>0.81100000000000005</v>
       </c>
-      <c r="S65" s="177">
+      <c r="S65" s="139">
         <v>343</v>
       </c>
-      <c r="T65" s="178" t="e">
+      <c r="T65" s="140" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="U65" s="178" t="e">
+      <c r="U65" s="140" t="e">
         <v>#VALUE!</v>
       </c>
       <c r="V65" s="1"/>
@@ -5798,7 +5798,7 @@
       <c r="E66" s="59">
         <v>1</v>
       </c>
-      <c r="F66" s="173">
+      <c r="F66" s="135">
         <v>44762</v>
       </c>
       <c r="G66" s="60">
@@ -5820,28 +5820,28 @@
       </c>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
-      <c r="N66" s="177">
+      <c r="N66" s="139">
         <v>0.75700000000000001</v>
       </c>
-      <c r="O66" s="177">
+      <c r="O66" s="139">
         <v>1.6459999999999999</v>
       </c>
-      <c r="P66" s="177">
+      <c r="P66" s="139">
         <v>0.58199999999999996</v>
       </c>
-      <c r="Q66" s="177">
+      <c r="Q66" s="139">
         <v>0.38200000000000001</v>
       </c>
-      <c r="R66" s="177">
+      <c r="R66" s="139">
         <v>0.82899999999999996</v>
       </c>
-      <c r="S66" s="177">
+      <c r="S66" s="139">
         <v>343</v>
       </c>
-      <c r="T66" s="177">
+      <c r="T66" s="139">
         <v>0.309</v>
       </c>
-      <c r="U66" s="177">
+      <c r="U66" s="139">
         <v>1.7284795770000001E-3</v>
       </c>
       <c r="V66" s="1"/>
@@ -5864,7 +5864,7 @@
       <c r="E67" s="59">
         <v>1</v>
       </c>
-      <c r="F67" s="173">
+      <c r="F67" s="135">
         <v>44762</v>
       </c>
       <c r="G67" s="60">
@@ -5886,28 +5886,28 @@
       </c>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
-      <c r="N67" s="177">
+      <c r="N67" s="139">
         <v>0.78200000000000003</v>
       </c>
-      <c r="O67" s="177">
+      <c r="O67" s="139">
         <v>1.657</v>
       </c>
-      <c r="P67" s="177">
+      <c r="P67" s="139">
         <v>0.57499999999999996</v>
       </c>
-      <c r="Q67" s="177">
+      <c r="Q67" s="139">
         <v>0.377</v>
       </c>
-      <c r="R67" s="177">
+      <c r="R67" s="139">
         <v>0.80100000000000005</v>
       </c>
-      <c r="S67" s="177">
+      <c r="S67" s="139">
         <v>343</v>
       </c>
-      <c r="T67" s="177">
+      <c r="T67" s="139">
         <v>0.317</v>
       </c>
-      <c r="U67" s="177">
+      <c r="U67" s="139">
         <v>2.1862586060000001E-3</v>
       </c>
       <c r="V67" s="1"/>
@@ -5930,7 +5930,7 @@
       <c r="E68" s="59">
         <v>1</v>
       </c>
-      <c r="F68" s="173">
+      <c r="F68" s="135">
         <v>44762</v>
       </c>
       <c r="G68" s="60">
@@ -5952,28 +5952,28 @@
       </c>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
-      <c r="N68" s="177" t="s">
+      <c r="N68" s="139" t="s">
         <v>411</v>
       </c>
-      <c r="O68" s="177">
+      <c r="O68" s="139">
         <v>1.508</v>
       </c>
-      <c r="P68" s="178" t="e">
+      <c r="P68" s="140" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="Q68" s="178" t="e">
+      <c r="Q68" s="140" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="R68" s="177">
+      <c r="R68" s="139">
         <v>0.72</v>
       </c>
-      <c r="S68" s="177">
+      <c r="S68" s="139">
         <v>343</v>
       </c>
-      <c r="T68" s="178" t="e">
+      <c r="T68" s="140" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="U68" s="178" t="e">
+      <c r="U68" s="140" t="e">
         <v>#VALUE!</v>
       </c>
       <c r="V68" s="1"/>
@@ -5996,7 +5996,7 @@
       <c r="E69" s="59">
         <v>1</v>
       </c>
-      <c r="F69" s="173">
+      <c r="F69" s="135">
         <v>44762</v>
       </c>
       <c r="G69" s="60">
@@ -6018,28 +6018,28 @@
       </c>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
-      <c r="N69" s="177">
+      <c r="N69" s="139">
         <v>0.76500000000000001</v>
       </c>
-      <c r="O69" s="177">
+      <c r="O69" s="139">
         <v>1.625</v>
       </c>
-      <c r="P69" s="177">
+      <c r="P69" s="139">
         <v>0.52200000000000002</v>
       </c>
-      <c r="Q69" s="177">
+      <c r="Q69" s="139">
         <v>0.34200000000000003</v>
       </c>
-      <c r="R69" s="177">
+      <c r="R69" s="139">
         <v>0.78200000000000003</v>
       </c>
-      <c r="S69" s="177">
+      <c r="S69" s="139">
         <v>343</v>
       </c>
-      <c r="T69" s="177">
+      <c r="T69" s="139">
         <v>0.38</v>
       </c>
-      <c r="U69" s="177">
+      <c r="U69" s="139">
         <v>2.9622584220000002E-3</v>
       </c>
       <c r="V69" s="1"/>
@@ -6062,7 +6062,7 @@
       <c r="E70" s="59">
         <v>1</v>
       </c>
-      <c r="F70" s="173">
+      <c r="F70" s="135">
         <v>44762</v>
       </c>
       <c r="G70" s="60">
@@ -6084,28 +6084,28 @@
       </c>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
-      <c r="N70" s="177">
+      <c r="N70" s="139">
         <v>0.77300000000000002</v>
       </c>
-      <c r="O70" s="177">
+      <c r="O70" s="139">
         <v>1.4710000000000001</v>
       </c>
-      <c r="P70" s="177">
+      <c r="P70" s="139">
         <v>0.58099999999999996</v>
       </c>
-      <c r="Q70" s="177">
+      <c r="Q70" s="139">
         <v>0.38100000000000001</v>
       </c>
-      <c r="R70" s="177">
+      <c r="R70" s="139">
         <v>0.73799999999999999</v>
       </c>
-      <c r="S70" s="177">
+      <c r="S70" s="139">
         <v>343</v>
       </c>
-      <c r="T70" s="177">
+      <c r="T70" s="139">
         <v>0.31</v>
       </c>
-      <c r="U70" s="177">
+      <c r="U70" s="139">
         <v>3.3948293279999998E-3</v>
       </c>
       <c r="V70" s="1"/>
@@ -6128,7 +6128,7 @@
       <c r="E71" s="59">
         <v>1</v>
       </c>
-      <c r="F71" s="173">
+      <c r="F71" s="135">
         <v>44761</v>
       </c>
       <c r="G71" s="60">
@@ -6150,28 +6150,28 @@
       </c>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
-      <c r="N71" s="177">
+      <c r="N71" s="139">
         <v>0.74299999999999999</v>
       </c>
-      <c r="O71" s="177">
+      <c r="O71" s="139">
         <v>1.538</v>
       </c>
-      <c r="P71" s="177">
+      <c r="P71" s="139">
         <v>0.57799999999999996</v>
       </c>
-      <c r="Q71" s="177">
+      <c r="Q71" s="139">
         <v>0.379</v>
       </c>
-      <c r="R71" s="177">
+      <c r="R71" s="139">
         <v>0.73599999999999999</v>
       </c>
-      <c r="S71" s="177">
+      <c r="S71" s="139">
         <v>344</v>
       </c>
-      <c r="T71" s="177">
+      <c r="T71" s="139">
         <v>0.314</v>
       </c>
-      <c r="U71" s="177">
+      <c r="U71" s="139">
         <v>3.4719792519999999E-3</v>
       </c>
       <c r="V71" s="1"/>
@@ -6194,7 +6194,7 @@
       <c r="E72" s="59">
         <v>1</v>
       </c>
-      <c r="F72" s="173">
+      <c r="F72" s="135">
         <v>44761</v>
       </c>
       <c r="G72" s="60">
@@ -6216,28 +6216,28 @@
       </c>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
-      <c r="N72" s="177" t="s">
+      <c r="N72" s="139" t="s">
         <v>411</v>
       </c>
-      <c r="O72" s="177">
+      <c r="O72" s="139">
         <v>1.504</v>
       </c>
-      <c r="P72" s="178" t="e">
+      <c r="P72" s="140" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="Q72" s="178" t="e">
+      <c r="Q72" s="140" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="R72" s="177">
+      <c r="R72" s="139">
         <v>0.70699999999999996</v>
       </c>
-      <c r="S72" s="177">
+      <c r="S72" s="139">
         <v>344</v>
       </c>
-      <c r="T72" s="178" t="e">
+      <c r="T72" s="140" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="U72" s="178" t="e">
+      <c r="U72" s="140" t="e">
         <v>#VALUE!</v>
       </c>
       <c r="V72" s="1"/>
@@ -6260,7 +6260,7 @@
       <c r="E73" s="59">
         <v>1</v>
       </c>
-      <c r="F73" s="173">
+      <c r="F73" s="135">
         <v>44761</v>
       </c>
       <c r="G73" s="60">
@@ -6282,28 +6282,28 @@
       </c>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
-      <c r="N73" s="177">
+      <c r="N73" s="139">
         <v>0.67200000000000004</v>
       </c>
-      <c r="O73" s="177">
+      <c r="O73" s="139">
         <v>1.6679999999999999</v>
       </c>
-      <c r="P73" s="177">
+      <c r="P73" s="139">
         <v>0.61</v>
       </c>
-      <c r="Q73" s="177">
+      <c r="Q73" s="139">
         <v>0.4</v>
       </c>
-      <c r="R73" s="177">
+      <c r="R73" s="139">
         <v>0.81200000000000006</v>
       </c>
-      <c r="S73" s="177">
+      <c r="S73" s="139">
         <v>344</v>
       </c>
-      <c r="T73" s="177">
+      <c r="T73" s="139">
         <v>0.27600000000000002</v>
       </c>
-      <c r="U73" s="177">
+      <c r="U73" s="139">
         <v>1.841943165E-3</v>
       </c>
       <c r="V73" s="1"/>
@@ -6326,7 +6326,7 @@
       <c r="E74" s="59">
         <v>1</v>
       </c>
-      <c r="F74" s="173">
+      <c r="F74" s="135">
         <v>44761</v>
       </c>
       <c r="G74" s="60">
@@ -6348,28 +6348,28 @@
       </c>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
-      <c r="N74" s="177">
+      <c r="N74" s="139">
         <v>0.69199999999999995</v>
       </c>
-      <c r="O74" s="177" t="s">
+      <c r="O74" s="139" t="s">
         <v>411</v>
       </c>
-      <c r="P74" s="177">
+      <c r="P74" s="139">
         <v>0.63200000000000001</v>
       </c>
-      <c r="Q74" s="177">
+      <c r="Q74" s="139">
         <v>0.41399999999999998</v>
       </c>
-      <c r="R74" s="178" t="e">
+      <c r="R74" s="140" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="S74" s="177">
+      <c r="S74" s="139">
         <v>344</v>
       </c>
-      <c r="T74" s="177">
+      <c r="T74" s="139">
         <v>0.249</v>
       </c>
-      <c r="U74" s="178" t="e">
+      <c r="U74" s="140" t="e">
         <v>#VALUE!</v>
       </c>
       <c r="V74" s="1"/>
@@ -6392,7 +6392,7 @@
       <c r="E75" s="59">
         <v>1</v>
       </c>
-      <c r="F75" s="173">
+      <c r="F75" s="135">
         <v>44761</v>
       </c>
       <c r="G75" s="60">
@@ -6414,28 +6414,28 @@
       </c>
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
-      <c r="N75" s="177">
+      <c r="N75" s="139">
         <v>0.78</v>
       </c>
-      <c r="O75" s="177">
+      <c r="O75" s="139">
         <v>1.556</v>
       </c>
-      <c r="P75" s="177">
+      <c r="P75" s="139">
         <v>0.57299999999999995</v>
       </c>
-      <c r="Q75" s="177">
+      <c r="Q75" s="139">
         <v>0.375</v>
       </c>
-      <c r="R75" s="177">
+      <c r="R75" s="139">
         <v>0.76900000000000002</v>
       </c>
-      <c r="S75" s="177">
+      <c r="S75" s="139">
         <v>344</v>
       </c>
-      <c r="T75" s="177">
+      <c r="T75" s="139">
         <v>0.32</v>
       </c>
-      <c r="U75" s="177">
+      <c r="U75" s="139">
         <v>2.775048768E-3</v>
       </c>
       <c r="V75" s="1"/>
@@ -6458,7 +6458,7 @@
       <c r="E76" s="59">
         <v>1</v>
       </c>
-      <c r="F76" s="173">
+      <c r="F76" s="135">
         <v>44761</v>
       </c>
       <c r="G76" s="60">
@@ -6480,28 +6480,28 @@
       </c>
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
-      <c r="N76" s="177">
+      <c r="N76" s="139">
         <v>0.77900000000000003</v>
       </c>
-      <c r="O76" s="177">
+      <c r="O76" s="139">
         <v>1.6639999999999999</v>
       </c>
-      <c r="P76" s="177">
+      <c r="P76" s="139">
         <v>0.56399999999999995</v>
       </c>
-      <c r="Q76" s="177">
+      <c r="Q76" s="139">
         <v>0.36899999999999999</v>
       </c>
-      <c r="R76" s="177">
+      <c r="R76" s="139">
         <v>0.79600000000000004</v>
       </c>
-      <c r="S76" s="177">
+      <c r="S76" s="139">
         <v>344</v>
       </c>
-      <c r="T76" s="177">
+      <c r="T76" s="139">
         <v>0.33100000000000002</v>
       </c>
-      <c r="U76" s="177">
+      <c r="U76" s="139">
         <v>2.3404909699999998E-3</v>
       </c>
       <c r="V76" s="1"/>
@@ -6524,7 +6524,7 @@
       <c r="E77" s="59">
         <v>1</v>
       </c>
-      <c r="F77" s="173">
+      <c r="F77" s="135">
         <v>44761</v>
       </c>
       <c r="G77" s="60">
@@ -6546,28 +6546,28 @@
       </c>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
-      <c r="N77" s="177">
+      <c r="N77" s="139">
         <v>0.747</v>
       </c>
-      <c r="O77" s="177">
+      <c r="O77" s="139">
         <v>1.5960000000000001</v>
       </c>
-      <c r="P77" s="177">
+      <c r="P77" s="139">
         <v>0.59599999999999997</v>
       </c>
-      <c r="Q77" s="177">
+      <c r="Q77" s="139">
         <v>0.39100000000000001</v>
       </c>
-      <c r="R77" s="177">
+      <c r="R77" s="139">
         <v>0.78900000000000003</v>
       </c>
-      <c r="S77" s="177">
+      <c r="S77" s="139">
         <v>344</v>
       </c>
-      <c r="T77" s="177">
+      <c r="T77" s="139">
         <v>0.29199999999999998</v>
       </c>
-      <c r="U77" s="177">
+      <c r="U77" s="139">
         <v>2.2620884309999998E-3</v>
       </c>
       <c r="V77" s="1"/>
@@ -6590,7 +6590,7 @@
       <c r="E78" s="59">
         <v>1</v>
       </c>
-      <c r="F78" s="173">
+      <c r="F78" s="135">
         <v>44761</v>
       </c>
       <c r="G78" s="60">
@@ -6612,28 +6612,28 @@
       </c>
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
-      <c r="N78" s="177">
+      <c r="N78" s="139">
         <v>0.73799999999999999</v>
       </c>
-      <c r="O78" s="177">
+      <c r="O78" s="139">
         <v>1.7010000000000001</v>
       </c>
-      <c r="P78" s="177">
+      <c r="P78" s="139">
         <v>0.58499999999999996</v>
       </c>
-      <c r="Q78" s="177">
+      <c r="Q78" s="139">
         <v>0.38300000000000001</v>
       </c>
-      <c r="R78" s="177">
+      <c r="R78" s="139">
         <v>0.82199999999999995</v>
       </c>
-      <c r="S78" s="177">
+      <c r="S78" s="139">
         <v>344</v>
       </c>
-      <c r="T78" s="177">
+      <c r="T78" s="139">
         <v>0.30599999999999999</v>
       </c>
-      <c r="U78" s="177">
+      <c r="U78" s="139">
         <v>1.8168674170000001E-3</v>
       </c>
       <c r="V78" s="1"/>
@@ -6656,7 +6656,7 @@
       <c r="E79" s="59">
         <v>1</v>
       </c>
-      <c r="F79" s="173">
+      <c r="F79" s="135">
         <v>44763</v>
       </c>
       <c r="G79" s="60">
@@ -6678,28 +6678,28 @@
       </c>
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
-      <c r="N79" s="177" t="s">
+      <c r="N79" s="139" t="s">
         <v>411</v>
       </c>
-      <c r="O79" s="177">
+      <c r="O79" s="139">
         <v>1.6120000000000001</v>
       </c>
-      <c r="P79" s="178" t="e">
+      <c r="P79" s="140" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="Q79" s="178" t="e">
+      <c r="Q79" s="140" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="R79" s="177">
+      <c r="R79" s="139">
         <v>0.78300000000000003</v>
       </c>
-      <c r="S79" s="177">
+      <c r="S79" s="139">
         <v>343</v>
       </c>
-      <c r="T79" s="178" t="e">
+      <c r="T79" s="140" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="U79" s="178" t="e">
+      <c r="U79" s="140" t="e">
         <v>#VALUE!</v>
       </c>
       <c r="V79" s="1"/>
@@ -6722,7 +6722,7 @@
       <c r="E80" s="59">
         <v>1</v>
       </c>
-      <c r="F80" s="173">
+      <c r="F80" s="135">
         <v>44763</v>
       </c>
       <c r="G80" s="60">
@@ -6744,28 +6744,28 @@
       </c>
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
-      <c r="N80" s="177">
+      <c r="N80" s="139">
         <v>0.83399999999999996</v>
       </c>
-      <c r="O80" s="177">
+      <c r="O80" s="139">
         <v>1.532</v>
       </c>
-      <c r="P80" s="177">
+      <c r="P80" s="139">
         <v>0.53500000000000003</v>
       </c>
-      <c r="Q80" s="177">
+      <c r="Q80" s="139">
         <v>0.35099999999999998</v>
       </c>
-      <c r="R80" s="177">
+      <c r="R80" s="139">
         <v>0.77400000000000002</v>
       </c>
-      <c r="S80" s="177">
+      <c r="S80" s="139">
         <v>343</v>
       </c>
-      <c r="T80" s="177">
+      <c r="T80" s="139">
         <v>0.36499999999999999</v>
       </c>
-      <c r="U80" s="177">
+      <c r="U80" s="139">
         <v>3.0189019510000002E-3</v>
       </c>
       <c r="V80" s="1"/>
@@ -6788,7 +6788,7 @@
       <c r="E81" s="59">
         <v>1</v>
       </c>
-      <c r="F81" s="173">
+      <c r="F81" s="135">
         <v>44763</v>
       </c>
       <c r="G81" s="60">
@@ -6810,28 +6810,28 @@
       </c>
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
-      <c r="N81" s="177">
+      <c r="N81" s="139">
         <v>0.89500000000000002</v>
       </c>
-      <c r="O81" s="177">
+      <c r="O81" s="139">
         <v>1.645</v>
       </c>
-      <c r="P81" s="177">
+      <c r="P81" s="139">
         <v>0.53700000000000003</v>
       </c>
-      <c r="Q81" s="177">
+      <c r="Q81" s="139">
         <v>0.35199999999999998</v>
       </c>
-      <c r="R81" s="177">
+      <c r="R81" s="139">
         <v>0.83499999999999996</v>
       </c>
-      <c r="S81" s="177">
+      <c r="S81" s="139">
         <v>343</v>
       </c>
-      <c r="T81" s="177">
+      <c r="T81" s="139">
         <v>0.36299999999999999</v>
       </c>
-      <c r="U81" s="177">
+      <c r="U81" s="139">
         <v>1.838416826E-3</v>
       </c>
       <c r="V81" s="1"/>
@@ -6854,7 +6854,7 @@
       <c r="E82" s="59">
         <v>1</v>
       </c>
-      <c r="F82" s="173">
+      <c r="F82" s="135">
         <v>44763</v>
       </c>
       <c r="G82" s="60">
@@ -6876,28 +6876,28 @@
       </c>
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
-      <c r="N82" s="177">
+      <c r="N82" s="139">
         <v>1.012</v>
       </c>
-      <c r="O82" s="177">
+      <c r="O82" s="139">
         <v>1.6220000000000001</v>
       </c>
-      <c r="P82" s="177">
+      <c r="P82" s="139">
         <v>0.43</v>
       </c>
-      <c r="Q82" s="177">
+      <c r="Q82" s="139">
         <v>0.28199999999999997</v>
       </c>
-      <c r="R82" s="177">
+      <c r="R82" s="139">
         <v>0.80400000000000005</v>
       </c>
-      <c r="S82" s="177">
+      <c r="S82" s="139">
         <v>343</v>
       </c>
-      <c r="T82" s="177">
+      <c r="T82" s="139">
         <v>0.48899999999999999</v>
       </c>
-      <c r="U82" s="177">
+      <c r="U82" s="139">
         <v>3.4553646650000002E-3</v>
       </c>
       <c r="V82" s="1"/>
@@ -6920,7 +6920,7 @@
       <c r="E83" s="59">
         <v>1</v>
       </c>
-      <c r="F83" s="173">
+      <c r="F83" s="135">
         <v>44763</v>
       </c>
       <c r="G83" s="60">
@@ -6942,28 +6942,28 @@
       </c>
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
-      <c r="N83" s="177">
+      <c r="N83" s="139">
         <v>0.874</v>
       </c>
-      <c r="O83" s="177">
+      <c r="O83" s="139">
         <v>1.581</v>
       </c>
-      <c r="P83" s="177">
+      <c r="P83" s="139">
         <v>0.52900000000000003</v>
       </c>
-      <c r="Q83" s="177">
+      <c r="Q83" s="139">
         <v>0.34699999999999998</v>
       </c>
-      <c r="R83" s="177">
+      <c r="R83" s="139">
         <v>0.78500000000000003</v>
       </c>
-      <c r="S83" s="177">
+      <c r="S83" s="139">
         <v>343</v>
       </c>
-      <c r="T83" s="177">
+      <c r="T83" s="139">
         <v>0.372</v>
       </c>
-      <c r="U83" s="177">
+      <c r="U83" s="139">
         <v>2.821044328E-3</v>
       </c>
       <c r="V83" s="1"/>
@@ -6986,7 +6986,7 @@
       <c r="E84" s="59">
         <v>1</v>
       </c>
-      <c r="F84" s="173">
+      <c r="F84" s="135">
         <v>44763</v>
       </c>
       <c r="G84" s="60">
@@ -7008,28 +7008,28 @@
       </c>
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
-      <c r="N84" s="177">
+      <c r="N84" s="139">
         <v>0.752</v>
       </c>
-      <c r="O84" s="177">
+      <c r="O84" s="139">
         <v>1.7070000000000001</v>
       </c>
-      <c r="P84" s="177">
+      <c r="P84" s="139">
         <v>0.58699999999999997</v>
       </c>
-      <c r="Q84" s="177">
+      <c r="Q84" s="139">
         <v>0.38500000000000001</v>
       </c>
-      <c r="R84" s="177">
+      <c r="R84" s="139">
         <v>0.83</v>
       </c>
-      <c r="S84" s="177">
+      <c r="S84" s="139">
         <v>343</v>
       </c>
-      <c r="T84" s="177">
+      <c r="T84" s="139">
         <v>0.30299999999999999</v>
       </c>
-      <c r="U84" s="177">
+      <c r="U84" s="139">
         <v>1.702975232E-3</v>
       </c>
       <c r="V84" s="1"/>
@@ -7052,7 +7052,7 @@
       <c r="E85" s="59">
         <v>1</v>
       </c>
-      <c r="F85" s="173">
+      <c r="F85" s="135">
         <v>44763</v>
       </c>
       <c r="G85" s="60">
@@ -7074,28 +7074,28 @@
       </c>
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
-      <c r="N85" s="177">
+      <c r="N85" s="139">
         <v>0.69099999999999995</v>
       </c>
-      <c r="O85" s="177">
+      <c r="O85" s="139">
         <v>1.6319999999999999</v>
       </c>
-      <c r="P85" s="177">
+      <c r="P85" s="139">
         <v>0.63800000000000001</v>
       </c>
-      <c r="Q85" s="177">
+      <c r="Q85" s="139">
         <v>0.41799999999999998</v>
       </c>
-      <c r="R85" s="177">
+      <c r="R85" s="139">
         <v>0.76600000000000001</v>
       </c>
-      <c r="S85" s="177">
+      <c r="S85" s="139">
         <v>343</v>
       </c>
-      <c r="T85" s="177">
+      <c r="T85" s="139">
         <v>0.24299999999999999</v>
       </c>
-      <c r="U85" s="177">
+      <c r="U85" s="139">
         <v>2.3864563549999998E-3</v>
       </c>
       <c r="V85" s="1"/>
@@ -7118,7 +7118,7 @@
       <c r="E86" s="59">
         <v>1</v>
       </c>
-      <c r="F86" s="173">
+      <c r="F86" s="135">
         <v>44763</v>
       </c>
       <c r="G86" s="60">
@@ -7140,28 +7140,28 @@
       </c>
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
-      <c r="N86" s="177">
+      <c r="N86" s="139">
         <v>0.753</v>
       </c>
-      <c r="O86" s="177">
+      <c r="O86" s="139">
         <v>1.605</v>
       </c>
-      <c r="P86" s="177">
+      <c r="P86" s="139">
         <v>0.59499999999999997</v>
       </c>
-      <c r="Q86" s="177">
+      <c r="Q86" s="139">
         <v>0.39</v>
       </c>
-      <c r="R86" s="177">
+      <c r="R86" s="139">
         <v>0.77200000000000002</v>
       </c>
-      <c r="S86" s="177">
+      <c r="S86" s="139">
         <v>343</v>
       </c>
-      <c r="T86" s="177">
+      <c r="T86" s="139">
         <v>0.29299999999999998</v>
       </c>
-      <c r="U86" s="177">
+      <c r="U86" s="139">
         <v>2.5514808530000001E-3</v>
       </c>
       <c r="V86" s="1"/>
@@ -7180,7 +7180,7 @@
         <v>117</v>
       </c>
       <c r="E87" s="59"/>
-      <c r="F87" s="174"/>
+      <c r="F87" s="136"/>
       <c r="G87" s="60">
         <v>2.0176400000000001</v>
       </c>
@@ -7240,7 +7240,7 @@
         <v>117</v>
       </c>
       <c r="E88" s="59"/>
-      <c r="F88" s="175"/>
+      <c r="F88" s="137"/>
       <c r="G88" s="3">
         <v>1.9499500000000001</v>
       </c>
@@ -7300,7 +7300,7 @@
         <v>117</v>
       </c>
       <c r="E89" s="59"/>
-      <c r="F89" s="176"/>
+      <c r="F89" s="138"/>
       <c r="G89" s="3">
         <v>2.1017299999999999</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>117</v>
       </c>
       <c r="E90" s="59"/>
-      <c r="F90" s="176"/>
+      <c r="F90" s="138"/>
       <c r="G90" s="3">
         <v>2.11707</v>
       </c>
@@ -7420,7 +7420,7 @@
         <v>117</v>
       </c>
       <c r="E91" s="59"/>
-      <c r="F91" s="176"/>
+      <c r="F91" s="138"/>
       <c r="G91" s="3">
         <v>2.0811000000000002</v>
       </c>
@@ -7480,7 +7480,7 @@
         <v>117</v>
       </c>
       <c r="E92" s="59"/>
-      <c r="F92" s="176"/>
+      <c r="F92" s="138"/>
       <c r="G92" s="3">
         <v>2.0568599999999999</v>
       </c>
@@ -35352,6 +35352,32 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="M39:T39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:F43"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="E44:F44"/>
     <mergeCell ref="B51:E51"/>
@@ -35366,32 +35392,6 @@
     <mergeCell ref="B47:D47"/>
     <mergeCell ref="E47:F47"/>
     <mergeCell ref="F51:K51"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="M39:T39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
   </mergeCells>
   <conditionalFormatting sqref="N59:U62 N87:U184">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
@@ -35440,8 +35440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>